<commit_message>
Updates to Weekly Report and Schedule
</commit_message>
<xml_diff>
--- a/Documents/Meeting Updates/Marching Masters Schedule.xlsx
+++ b/Documents/Meeting Updates/Marching Masters Schedule.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{60E66C40-4F07-1A4A-8C0F-970721A7FFDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF7EE4E-CC0C-484B-9978-8398BD2DE522}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13749" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="11" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="65">
   <si>
     <t>About This Template</t>
   </si>
@@ -241,6 +241,18 @@
   </si>
   <si>
     <t>Low</t>
+  </si>
+  <si>
+    <t>Adam, Tumaris</t>
+  </si>
+  <si>
+    <t>Jeffer, Brandin</t>
+  </si>
+  <si>
+    <t>Aparna, Siddharth</t>
+  </si>
+  <si>
+    <t>Aparna, Brandin</t>
   </si>
 </sst>
 </file>
@@ -750,6 +762,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -766,28 +793,13 @@
     <xf numFmtId="14" fontId="6" fillId="0" borderId="7" xfId="9" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="11" xfId="9" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="8" xfId="9" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="11" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="11" xfId="9" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -806,6 +818,79 @@
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
   <dxfs count="26">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="2" tint="-9.9948118533890809E-2"/>
+        </left>
+        <right style="thin">
+          <color theme="2" tint="-9.9948118533890809E-2"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -893,46 +978,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="2" tint="-9.9948118533890809E-2"/>
-        </left>
-        <right style="thin">
-          <color theme="2" tint="-9.9948118533890809E-2"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="6" tint="0.59996337778862885"/>
@@ -995,39 +1040,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border>
@@ -1291,15 +1303,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>25400</xdr:colOff>
+          <xdr:colOff>23854</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>63500</xdr:rowOff>
+          <xdr:rowOff>63610</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>84</xdr:col>
-          <xdr:colOff>75052</xdr:colOff>
+          <xdr:colOff>127221</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>241300</xdr:rowOff>
+          <xdr:rowOff>238539</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1351,12 +1363,12 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{EE48C34E-B98C-4BBA-90C8-388E8655DD6D}" name="Milestone Description" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{B8ACC97F-C189-49BA-91CF-CB5671185BCF}" name="Category" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{5419FA1B-A035-4F0A-9257-1AA4BCB5E6CF}" name="Assigned To" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{EE48C34E-B98C-4BBA-90C8-388E8655DD6D}" name="Milestone Description" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{B8ACC97F-C189-49BA-91CF-CB5671185BCF}" name="Category" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{5419FA1B-A035-4F0A-9257-1AA4BCB5E6CF}" name="Assigned To" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{A60A6524-18F0-48B7-BB3C-2F4A35799FF7}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{59612C1F-9AAB-483B-A6A5-3563E9D77941}" name="Start" dataCellStyle="Date"/>
-    <tableColumn id="7" xr3:uid="{FFB4566D-F84D-4445-98D2-EC6DB0387316}" name="End" dataDxfId="10" dataCellStyle="Date"/>
+    <tableColumn id="7" xr3:uid="{FFB4566D-F84D-4445-98D2-EC6DB0387316}" name="End" dataDxfId="0" dataCellStyle="Date"/>
     <tableColumn id="6" xr3:uid="{012C59F1-49D4-4A67-B8DD-855C6581FD6A}" name="No. Days" dataCellStyle="Comma [0]"/>
   </tableColumns>
   <tableStyleInfo name="Gantt Table Style" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1636,24 +1648,24 @@
   </sheetPr>
   <dimension ref="A1:CA127"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A4" zoomScale="139" zoomScaleNormal="150" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="30.05" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.6640625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" customWidth="1"/>
-    <col min="3" max="3" width="10.5" style="20" customWidth="1"/>
-    <col min="4" max="4" width="20.5" customWidth="1"/>
+    <col min="2" max="2" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" customWidth="1"/>
-    <col min="6" max="7" width="10.5" style="3" customWidth="1"/>
-    <col min="8" max="8" width="10.5" customWidth="1"/>
+    <col min="6" max="7" width="10.44140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="10.44140625" customWidth="1"/>
     <col min="9" max="9" width="2.6640625" customWidth="1"/>
-    <col min="10" max="83" width="2.5" customWidth="1"/>
+    <col min="10" max="83" width="2.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:79" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:79" ht="30.05" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="15" t="s">
         <v>23</v>
       </c>
@@ -1693,7 +1705,7 @@
       <c r="AG1" s="20"/>
       <c r="AH1" s="20"/>
     </row>
-    <row r="2" spans="1:79" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:79" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="15" t="s">
         <v>15</v>
       </c>
@@ -1704,80 +1716,80 @@
       <c r="F2" s="23"/>
       <c r="G2" s="23"/>
       <c r="H2" s="21"/>
-      <c r="J2" s="54" t="s">
+      <c r="J2" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="Q2" s="55" t="s">
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="60"/>
+      <c r="N2" s="60"/>
+      <c r="O2" s="60"/>
+      <c r="Q2" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="R2" s="55"/>
-      <c r="S2" s="55"/>
-      <c r="T2" s="55"/>
-      <c r="U2" s="55"/>
-      <c r="V2" s="55"/>
-      <c r="X2" s="56" t="s">
+      <c r="R2" s="50"/>
+      <c r="S2" s="50"/>
+      <c r="T2" s="50"/>
+      <c r="U2" s="50"/>
+      <c r="V2" s="50"/>
+      <c r="X2" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="Y2" s="56"/>
-      <c r="Z2" s="56"/>
-      <c r="AA2" s="56"/>
-      <c r="AB2" s="56"/>
-      <c r="AC2" s="56"/>
-      <c r="AE2" s="47" t="s">
+      <c r="Y2" s="51"/>
+      <c r="Z2" s="51"/>
+      <c r="AA2" s="51"/>
+      <c r="AB2" s="51"/>
+      <c r="AC2" s="51"/>
+      <c r="AE2" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="AF2" s="47"/>
-      <c r="AG2" s="47"/>
-      <c r="AH2" s="47"/>
-      <c r="AI2" s="47"/>
-      <c r="AJ2" s="47"/>
-      <c r="AL2" s="48" t="s">
+      <c r="AF2" s="52"/>
+      <c r="AG2" s="52"/>
+      <c r="AH2" s="52"/>
+      <c r="AI2" s="52"/>
+      <c r="AJ2" s="52"/>
+      <c r="AL2" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="AM2" s="48"/>
-      <c r="AN2" s="48"/>
-      <c r="AO2" s="48"/>
-      <c r="AP2" s="48"/>
-      <c r="AQ2" s="48"/>
+      <c r="AM2" s="53"/>
+      <c r="AN2" s="53"/>
+      <c r="AO2" s="53"/>
+      <c r="AP2" s="53"/>
+      <c r="AQ2" s="53"/>
       <c r="AR2" s="20"/>
       <c r="AW2" s="20"/>
       <c r="BB2" s="20"/>
     </row>
-    <row r="3" spans="1:79" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:79" ht="30.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="50"/>
-      <c r="F3" s="52">
+      <c r="E3" s="55"/>
+      <c r="F3" s="57">
         <f ca="1">IFERROR(IF(MIN(Milestones[Start])=0,TODAY(),MIN(Milestones[Start])),TODAY())</f>
         <v>44096</v>
       </c>
-      <c r="G3" s="57"/>
-      <c r="H3" s="53"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="59"/>
       <c r="I3" s="22"/>
     </row>
-    <row r="4" spans="1:79" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:79" ht="30.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="49" t="s">
+      <c r="D4" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="50"/>
+      <c r="E4" s="55"/>
       <c r="F4" s="39">
         <v>0</v>
       </c>
-      <c r="G4" s="58"/>
+      <c r="G4" s="47"/>
       <c r="J4" s="38" t="str">
         <f ca="1">TEXT(J5,"mmmm")</f>
         <v>September</v>
@@ -1873,18 +1885,18 @@
       <c r="BZ4" s="38"/>
       <c r="CA4" s="38"/>
     </row>
-    <row r="5" spans="1:79" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:79" ht="15.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="51"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="51"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="56"/>
+      <c r="H5" s="56"/>
+      <c r="I5" s="56"/>
       <c r="J5" s="43">
         <f ca="1">IFERROR(Project_Start+Scrolling_Increment,TODAY())</f>
         <v>44096</v>
@@ -2166,7 +2178,7 @@
         <v>44165</v>
       </c>
     </row>
-    <row r="6" spans="1:79" s="20" customFormat="1" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:79" s="20" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>18</v>
       </c>
@@ -2249,7 +2261,7 @@
       <c r="BZ6" s="42"/>
       <c r="CA6" s="42"/>
     </row>
-    <row r="7" spans="1:79" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:79" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="15" t="s">
         <v>19</v>
       </c>
@@ -2556,16 +2568,14 @@
         <v>M</v>
       </c>
     </row>
-    <row r="8" spans="1:79" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:79" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="32" t="s">
-        <v>57</v>
-      </c>
+      <c r="C8" s="32"/>
       <c r="D8" s="32"/>
       <c r="E8" s="29">
         <v>0</v>
@@ -2862,7 +2872,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:79" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:79" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15"/>
       <c r="B9" s="36" t="s">
         <v>27</v>
@@ -3168,7 +3178,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:79" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:79" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="15"/>
       <c r="B10" s="36" t="s">
         <v>28</v>
@@ -3180,7 +3190,7 @@
         <v>33</v>
       </c>
       <c r="E10" s="29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="30">
         <v>44108</v>
@@ -3474,7 +3484,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:79" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:79" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15"/>
       <c r="B11" s="37" t="s">
         <v>40</v>
@@ -3767,7 +3777,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:79" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:79" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15"/>
       <c r="B12" s="36" t="s">
         <v>36</v>
@@ -3775,7 +3785,9 @@
       <c r="C12" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="60"/>
+      <c r="D12" s="49" t="s">
+        <v>63</v>
+      </c>
       <c r="E12" s="29">
         <v>0.15</v>
       </c>
@@ -4071,7 +4083,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:79" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:79" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="B13" s="36" t="s">
         <v>37</v>
@@ -4079,7 +4091,7 @@
       <c r="C13" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="60"/>
+      <c r="D13" s="49"/>
       <c r="E13" s="29">
         <v>0</v>
       </c>
@@ -4095,227 +4107,227 @@
       </c>
       <c r="I13" s="25"/>
       <c r="J13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",J$5&gt;=$F13,J$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",J$5&gt;=$F13,J$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ref="J13:S17" ca="1" si="30">IF(AND($C13="Goal",J$5&gt;=$F13,J$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",J$5&gt;=$F13,J$5&lt;=$F13+$H13-1),1,""))</f>
         <v/>
       </c>
       <c r="K13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",K$5&gt;=$F13,K$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",K$5&gt;=$F13,K$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="L13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",L$5&gt;=$F13,L$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",L$5&gt;=$F13,L$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="M13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",M$5&gt;=$F13,M$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",M$5&gt;=$F13,M$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="N13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",N$5&gt;=$F13,N$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",N$5&gt;=$F13,N$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="O13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",O$5&gt;=$F13,O$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",O$5&gt;=$F13,O$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="P13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",P$5&gt;=$F13,P$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",P$5&gt;=$F13,P$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="Q13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",Q$5&gt;=$F13,Q$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",Q$5&gt;=$F13,Q$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="R13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",R$5&gt;=$F13,R$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",R$5&gt;=$F13,R$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="S13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",S$5&gt;=$F13,S$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",S$5&gt;=$F13,S$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="T13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",T$5&gt;=$F13,T$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",T$5&gt;=$F13,T$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="24"/>
         <v/>
       </c>
       <c r="U13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",U$5&gt;=$F13,U$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",U$5&gt;=$F13,U$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="24"/>
         <v/>
       </c>
       <c r="V13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",V$5&gt;=$F13,V$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",V$5&gt;=$F13,V$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="24"/>
         <v/>
       </c>
       <c r="W13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",W$5&gt;=$F13,W$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",W$5&gt;=$F13,W$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="24"/>
         <v/>
       </c>
       <c r="X13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",X$5&gt;=$F13,X$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",X$5&gt;=$F13,X$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="24"/>
         <v/>
       </c>
       <c r="Y13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",Y$5&gt;=$F13,Y$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",Y$5&gt;=$F13,Y$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="24"/>
         <v/>
       </c>
       <c r="Z13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",Z$5&gt;=$F13,Z$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",Z$5&gt;=$F13,Z$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AA13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",AA$5&gt;=$F13,AA$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",AA$5&gt;=$F13,AA$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AB13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",AB$5&gt;=$F13,AB$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",AB$5&gt;=$F13,AB$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AC13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",AC$5&gt;=$F13,AC$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",AC$5&gt;=$F13,AC$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AD13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",AD$5&gt;=$F13,AD$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",AD$5&gt;=$F13,AD$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AE13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",AE$5&gt;=$F13,AE$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",AE$5&gt;=$F13,AE$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AF13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",AF$5&gt;=$F13,AF$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",AF$5&gt;=$F13,AF$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AG13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",AG$5&gt;=$F13,AG$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",AG$5&gt;=$F13,AG$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AH13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",AH$5&gt;=$F13,AH$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",AH$5&gt;=$F13,AH$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AI13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",AI$5&gt;=$F13,AI$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",AI$5&gt;=$F13,AI$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AJ13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",AJ$5&gt;=$F13,AJ$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",AJ$5&gt;=$F13,AJ$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AK13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",AK$5&gt;=$F13,AK$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",AK$5&gt;=$F13,AK$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AL13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",AL$5&gt;=$F13,AL$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",AL$5&gt;=$F13,AL$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AM13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",AM$5&gt;=$F13,AM$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",AM$5&gt;=$F13,AM$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AN13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",AN$5&gt;=$F13,AN$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",AN$5&gt;=$F13,AN$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AO13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",AO$5&gt;=$F13,AO$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",AO$5&gt;=$F13,AO$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AP13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",AP$5&gt;=$F13,AP$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",AP$5&gt;=$F13,AP$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AQ13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",AQ$5&gt;=$F13,AQ$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",AQ$5&gt;=$F13,AQ$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AR13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",AR$5&gt;=$F13,AR$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",AR$5&gt;=$F13,AR$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AS13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",AS$5&gt;=$F13,AS$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",AS$5&gt;=$F13,AS$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AT13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",AT$5&gt;=$F13,AT$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",AT$5&gt;=$F13,AT$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AU13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",AU$5&gt;=$F13,AU$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",AU$5&gt;=$F13,AU$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AV13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",AV$5&gt;=$F13,AV$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",AV$5&gt;=$F13,AV$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AW13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",AW$5&gt;=$F13,AW$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",AW$5&gt;=$F13,AW$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AX13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",AX$5&gt;=$F13,AX$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",AX$5&gt;=$F13,AX$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AY13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",AY$5&gt;=$F13,AY$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",AY$5&gt;=$F13,AY$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AZ13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",AZ$5&gt;=$F13,AZ$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",AZ$5&gt;=$F13,AZ$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="BA13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",BA$5&gt;=$F13,BA$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",BA$5&gt;=$F13,BA$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="BB13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",BB$5&gt;=$F13,BB$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",BB$5&gt;=$F13,BB$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="BC13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",BC$5&gt;=$F13,BC$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",BC$5&gt;=$F13,BC$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="BD13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",BD$5&gt;=$F13,BD$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",BD$5&gt;=$F13,BD$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="BE13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",BE$5&gt;=$F13,BE$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",BE$5&gt;=$F13,BE$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="BF13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",BF$5&gt;=$F13,BF$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",BF$5&gt;=$F13,BF$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BG13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",BG$5&gt;=$F13,BG$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",BG$5&gt;=$F13,BG$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BH13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",BH$5&gt;=$F13,BH$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",BH$5&gt;=$F13,BH$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BI13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",BI$5&gt;=$F13,BI$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",BI$5&gt;=$F13,BI$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BJ13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",BJ$5&gt;=$F13,BJ$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",BJ$5&gt;=$F13,BJ$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BK13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",BK$5&gt;=$F13,BK$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",BK$5&gt;=$F13,BK$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BL13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",BL$5&gt;=$F13,BL$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",BL$5&gt;=$F13,BL$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BM13" s="34" t="str">
-        <f ca="1">IF(AND($C13="Goal",BM$5&gt;=$F13,BM$5&lt;=$F13+$H13-1),2,IF(AND($C13="Milestone",BM$5&gt;=$F13,BM$5&lt;=$F13+$H13-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BN13" s="34" t="str">
@@ -4375,7 +4387,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:79" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:79" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="37" t="s">
         <v>30</v>
@@ -4391,287 +4403,287 @@
       </c>
       <c r="I14" s="25"/>
       <c r="J14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",J$5&gt;=$F14,J$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",J$5&gt;=$F14,J$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="K14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",K$5&gt;=$F14,K$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",K$5&gt;=$F14,K$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="L14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",L$5&gt;=$F14,L$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",L$5&gt;=$F14,L$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="M14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",M$5&gt;=$F14,M$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",M$5&gt;=$F14,M$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="N14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",N$5&gt;=$F14,N$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",N$5&gt;=$F14,N$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="O14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",O$5&gt;=$F14,O$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",O$5&gt;=$F14,O$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="P14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",P$5&gt;=$F14,P$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",P$5&gt;=$F14,P$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="Q14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",Q$5&gt;=$F14,Q$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",Q$5&gt;=$F14,Q$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="R14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",R$5&gt;=$F14,R$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",R$5&gt;=$F14,R$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="S14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",S$5&gt;=$F14,S$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",S$5&gt;=$F14,S$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="T14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",T$5&gt;=$F14,T$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",T$5&gt;=$F14,T$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="24"/>
         <v/>
       </c>
       <c r="U14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",U$5&gt;=$F14,U$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",U$5&gt;=$F14,U$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="24"/>
         <v/>
       </c>
       <c r="V14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",V$5&gt;=$F14,V$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",V$5&gt;=$F14,V$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="24"/>
         <v/>
       </c>
       <c r="W14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",W$5&gt;=$F14,W$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",W$5&gt;=$F14,W$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="24"/>
         <v/>
       </c>
       <c r="X14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",X$5&gt;=$F14,X$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",X$5&gt;=$F14,X$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="24"/>
         <v/>
       </c>
       <c r="Y14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",Y$5&gt;=$F14,Y$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",Y$5&gt;=$F14,Y$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="24"/>
         <v/>
       </c>
       <c r="Z14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",Z$5&gt;=$F14,Z$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",Z$5&gt;=$F14,Z$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AA14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",AA$5&gt;=$F14,AA$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",AA$5&gt;=$F14,AA$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AB14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",AB$5&gt;=$F14,AB$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",AB$5&gt;=$F14,AB$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AC14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",AC$5&gt;=$F14,AC$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",AC$5&gt;=$F14,AC$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AD14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",AD$5&gt;=$F14,AD$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",AD$5&gt;=$F14,AD$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AE14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",AE$5&gt;=$F14,AE$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",AE$5&gt;=$F14,AE$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AF14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",AF$5&gt;=$F14,AF$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",AF$5&gt;=$F14,AF$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AG14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",AG$5&gt;=$F14,AG$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",AG$5&gt;=$F14,AG$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AH14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",AH$5&gt;=$F14,AH$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",AH$5&gt;=$F14,AH$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AI14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",AI$5&gt;=$F14,AI$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",AI$5&gt;=$F14,AI$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AJ14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",AJ$5&gt;=$F14,AJ$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",AJ$5&gt;=$F14,AJ$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AK14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",AK$5&gt;=$F14,AK$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",AK$5&gt;=$F14,AK$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AL14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",AL$5&gt;=$F14,AL$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",AL$5&gt;=$F14,AL$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AM14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",AM$5&gt;=$F14,AM$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",AM$5&gt;=$F14,AM$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AN14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",AN$5&gt;=$F14,AN$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",AN$5&gt;=$F14,AN$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AO14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",AO$5&gt;=$F14,AO$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",AO$5&gt;=$F14,AO$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AP14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",AP$5&gt;=$F14,AP$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",AP$5&gt;=$F14,AP$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AQ14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",AQ$5&gt;=$F14,AQ$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",AQ$5&gt;=$F14,AQ$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AR14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",AR$5&gt;=$F14,AR$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",AR$5&gt;=$F14,AR$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AS14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",AS$5&gt;=$F14,AS$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",AS$5&gt;=$F14,AS$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AT14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",AT$5&gt;=$F14,AT$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",AT$5&gt;=$F14,AT$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AU14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",AU$5&gt;=$F14,AU$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",AU$5&gt;=$F14,AU$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AV14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",AV$5&gt;=$F14,AV$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",AV$5&gt;=$F14,AV$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AW14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",AW$5&gt;=$F14,AW$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",AW$5&gt;=$F14,AW$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AX14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",AX$5&gt;=$F14,AX$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",AX$5&gt;=$F14,AX$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AY14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",AY$5&gt;=$F14,AY$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",AY$5&gt;=$F14,AY$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AZ14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",AZ$5&gt;=$F14,AZ$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",AZ$5&gt;=$F14,AZ$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="BA14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",BA$5&gt;=$F14,BA$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",BA$5&gt;=$F14,BA$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="BB14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",BB$5&gt;=$F14,BB$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",BB$5&gt;=$F14,BB$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="BC14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",BC$5&gt;=$F14,BC$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",BC$5&gt;=$F14,BC$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="BD14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",BD$5&gt;=$F14,BD$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",BD$5&gt;=$F14,BD$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="BE14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",BE$5&gt;=$F14,BE$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",BE$5&gt;=$F14,BE$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="BF14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",BF$5&gt;=$F14,BF$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",BF$5&gt;=$F14,BF$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BG14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",BG$5&gt;=$F14,BG$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",BG$5&gt;=$F14,BG$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BH14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",BH$5&gt;=$F14,BH$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",BH$5&gt;=$F14,BH$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BI14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",BI$5&gt;=$F14,BI$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",BI$5&gt;=$F14,BI$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BJ14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",BJ$5&gt;=$F14,BJ$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",BJ$5&gt;=$F14,BJ$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BK14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",BK$5&gt;=$F14,BK$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",BK$5&gt;=$F14,BK$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BL14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",BL$5&gt;=$F14,BL$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",BL$5&gt;=$F14,BL$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BM14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",BM$5&gt;=$F14,BM$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",BM$5&gt;=$F14,BM$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BN14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",BN$5&gt;=$F14,BN$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",BN$5&gt;=$F14,BN$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ref="BN14:CA17" ca="1" si="31">IF(AND($C14="Goal",BN$5&gt;=$F14,BN$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",BN$5&gt;=$F14,BN$5&lt;=$F14+$H14-1),1,""))</f>
         <v/>
       </c>
       <c r="BO14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",BO$5&gt;=$F14,BO$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",BO$5&gt;=$F14,BO$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BP14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",BP$5&gt;=$F14,BP$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",BP$5&gt;=$F14,BP$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BQ14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",BQ$5&gt;=$F14,BQ$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",BQ$5&gt;=$F14,BQ$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BR14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",BR$5&gt;=$F14,BR$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",BR$5&gt;=$F14,BR$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BS14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",BS$5&gt;=$F14,BS$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",BS$5&gt;=$F14,BS$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BT14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",BT$5&gt;=$F14,BT$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",BT$5&gt;=$F14,BT$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BU14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",BU$5&gt;=$F14,BU$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",BU$5&gt;=$F14,BU$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BV14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",BV$5&gt;=$F14,BV$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",BV$5&gt;=$F14,BV$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BW14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",BW$5&gt;=$F14,BW$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",BW$5&gt;=$F14,BW$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BX14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",BX$5&gt;=$F14,BX$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",BX$5&gt;=$F14,BX$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BY14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",BY$5&gt;=$F14,BY$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",BY$5&gt;=$F14,BY$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BZ14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",BZ$5&gt;=$F14,BZ$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",BZ$5&gt;=$F14,BZ$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="CA14" s="34" t="str">
-        <f ca="1">IF(AND($C14="Goal",CA$5&gt;=$F14,CA$5&lt;=$F14+$H14-1),2,IF(AND($C14="Milestone",CA$5&gt;=$F14,CA$5&lt;=$F14+$H14-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:79" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:79" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="36" t="s">
         <v>47</v>
@@ -4679,303 +4691,305 @@
       <c r="C15" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="60"/>
+      <c r="D15" s="49" t="s">
+        <v>62</v>
+      </c>
       <c r="E15" s="29">
         <v>0</v>
       </c>
       <c r="F15" s="30">
-        <v>44103</v>
+        <v>44110</v>
       </c>
       <c r="G15" s="30">
         <v>44131</v>
       </c>
       <c r="H15" s="31">
         <f>Milestones[[#This Row],[End]]-Milestones[[#This Row],[Start]]+1</f>
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="I15" s="25"/>
       <c r="J15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",J$5&gt;=$F15,J$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",J$5&gt;=$F15,J$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="K15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",K$5&gt;=$F15,K$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",K$5&gt;=$F15,K$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="L15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",L$5&gt;=$F15,L$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",L$5&gt;=$F15,L$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="M15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",M$5&gt;=$F15,M$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",M$5&gt;=$F15,M$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="N15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",N$5&gt;=$F15,N$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",N$5&gt;=$F15,N$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="O15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",O$5&gt;=$F15,O$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",O$5&gt;=$F15,O$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="P15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",P$5&gt;=$F15,P$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",P$5&gt;=$F15,P$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="Q15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",Q$5&gt;=$F15,Q$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",Q$5&gt;=$F15,Q$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="R15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",R$5&gt;=$F15,R$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",R$5&gt;=$F15,R$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="S15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",S$5&gt;=$F15,S$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",S$5&gt;=$F15,S$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="T15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",T$5&gt;=$F15,T$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",T$5&gt;=$F15,T$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="24"/>
         <v/>
       </c>
       <c r="U15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",U$5&gt;=$F15,U$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",U$5&gt;=$F15,U$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="24"/>
         <v/>
       </c>
       <c r="V15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",V$5&gt;=$F15,V$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",V$5&gt;=$F15,V$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="24"/>
         <v/>
       </c>
       <c r="W15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",W$5&gt;=$F15,W$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",W$5&gt;=$F15,W$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="24"/>
         <v/>
       </c>
       <c r="X15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",X$5&gt;=$F15,X$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",X$5&gt;=$F15,X$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="24"/>
         <v/>
       </c>
       <c r="Y15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",Y$5&gt;=$F15,Y$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",Y$5&gt;=$F15,Y$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="24"/>
         <v/>
       </c>
       <c r="Z15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",Z$5&gt;=$F15,Z$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",Z$5&gt;=$F15,Z$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AA15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",AA$5&gt;=$F15,AA$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",AA$5&gt;=$F15,AA$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AB15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",AB$5&gt;=$F15,AB$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",AB$5&gt;=$F15,AB$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AC15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",AC$5&gt;=$F15,AC$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",AC$5&gt;=$F15,AC$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AD15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",AD$5&gt;=$F15,AD$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",AD$5&gt;=$F15,AD$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AE15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",AE$5&gt;=$F15,AE$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",AE$5&gt;=$F15,AE$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AF15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",AF$5&gt;=$F15,AF$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",AF$5&gt;=$F15,AF$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AG15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",AG$5&gt;=$F15,AG$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",AG$5&gt;=$F15,AG$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AH15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",AH$5&gt;=$F15,AH$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",AH$5&gt;=$F15,AH$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AI15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",AI$5&gt;=$F15,AI$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",AI$5&gt;=$F15,AI$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AJ15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",AJ$5&gt;=$F15,AJ$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",AJ$5&gt;=$F15,AJ$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AK15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",AK$5&gt;=$F15,AK$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",AK$5&gt;=$F15,AK$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AL15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",AL$5&gt;=$F15,AL$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",AL$5&gt;=$F15,AL$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AM15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",AM$5&gt;=$F15,AM$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",AM$5&gt;=$F15,AM$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AN15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",AN$5&gt;=$F15,AN$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",AN$5&gt;=$F15,AN$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AO15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",AO$5&gt;=$F15,AO$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",AO$5&gt;=$F15,AO$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AP15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",AP$5&gt;=$F15,AP$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",AP$5&gt;=$F15,AP$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AQ15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",AQ$5&gt;=$F15,AQ$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",AQ$5&gt;=$F15,AQ$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AR15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",AR$5&gt;=$F15,AR$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",AR$5&gt;=$F15,AR$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AS15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",AS$5&gt;=$F15,AS$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",AS$5&gt;=$F15,AS$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AT15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",AT$5&gt;=$F15,AT$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",AT$5&gt;=$F15,AT$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AU15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",AU$5&gt;=$F15,AU$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",AU$5&gt;=$F15,AU$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AV15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",AV$5&gt;=$F15,AV$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",AV$5&gt;=$F15,AV$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AW15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",AW$5&gt;=$F15,AW$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",AW$5&gt;=$F15,AW$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AX15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",AX$5&gt;=$F15,AX$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",AX$5&gt;=$F15,AX$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AY15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",AY$5&gt;=$F15,AY$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",AY$5&gt;=$F15,AY$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AZ15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",AZ$5&gt;=$F15,AZ$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",AZ$5&gt;=$F15,AZ$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="BA15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",BA$5&gt;=$F15,BA$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",BA$5&gt;=$F15,BA$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="BB15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",BB$5&gt;=$F15,BB$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",BB$5&gt;=$F15,BB$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="BC15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",BC$5&gt;=$F15,BC$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",BC$5&gt;=$F15,BC$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="BD15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",BD$5&gt;=$F15,BD$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",BD$5&gt;=$F15,BD$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="BE15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",BE$5&gt;=$F15,BE$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",BE$5&gt;=$F15,BE$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="BF15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",BF$5&gt;=$F15,BF$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",BF$5&gt;=$F15,BF$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BG15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",BG$5&gt;=$F15,BG$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",BG$5&gt;=$F15,BG$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BH15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",BH$5&gt;=$F15,BH$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",BH$5&gt;=$F15,BH$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BI15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",BI$5&gt;=$F15,BI$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",BI$5&gt;=$F15,BI$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BJ15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",BJ$5&gt;=$F15,BJ$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",BJ$5&gt;=$F15,BJ$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BK15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",BK$5&gt;=$F15,BK$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",BK$5&gt;=$F15,BK$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BL15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",BL$5&gt;=$F15,BL$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",BL$5&gt;=$F15,BL$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BM15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",BM$5&gt;=$F15,BM$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",BM$5&gt;=$F15,BM$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BN15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",BN$5&gt;=$F15,BN$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",BN$5&gt;=$F15,BN$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BO15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",BO$5&gt;=$F15,BO$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",BO$5&gt;=$F15,BO$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BP15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",BP$5&gt;=$F15,BP$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",BP$5&gt;=$F15,BP$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BQ15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",BQ$5&gt;=$F15,BQ$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",BQ$5&gt;=$F15,BQ$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BR15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",BR$5&gt;=$F15,BR$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",BR$5&gt;=$F15,BR$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BS15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",BS$5&gt;=$F15,BS$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",BS$5&gt;=$F15,BS$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BT15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",BT$5&gt;=$F15,BT$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",BT$5&gt;=$F15,BT$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BU15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",BU$5&gt;=$F15,BU$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",BU$5&gt;=$F15,BU$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BV15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",BV$5&gt;=$F15,BV$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",BV$5&gt;=$F15,BV$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BW15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",BW$5&gt;=$F15,BW$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",BW$5&gt;=$F15,BW$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BX15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",BX$5&gt;=$F15,BX$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",BX$5&gt;=$F15,BX$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BY15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",BY$5&gt;=$F15,BY$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",BY$5&gt;=$F15,BY$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BZ15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",BZ$5&gt;=$F15,BZ$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",BZ$5&gt;=$F15,BZ$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="CA15" s="34" t="str">
-        <f ca="1">IF(AND($C15="Goal",CA$5&gt;=$F15,CA$5&lt;=$F15+$H15-1),2,IF(AND($C15="Milestone",CA$5&gt;=$F15,CA$5&lt;=$F15+$H15-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:79" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:79" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="36" t="s">
         <v>38</v>
@@ -4983,7 +4997,7 @@
       <c r="C16" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="60"/>
+      <c r="D16" s="49"/>
       <c r="E16" s="29">
         <v>0</v>
       </c>
@@ -4999,287 +5013,287 @@
       </c>
       <c r="I16" s="25"/>
       <c r="J16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",J$5&gt;=$F16,J$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",J$5&gt;=$F16,J$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="K16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",K$5&gt;=$F16,K$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",K$5&gt;=$F16,K$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="L16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",L$5&gt;=$F16,L$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",L$5&gt;=$F16,L$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="M16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",M$5&gt;=$F16,M$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",M$5&gt;=$F16,M$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="N16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",N$5&gt;=$F16,N$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",N$5&gt;=$F16,N$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="O16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",O$5&gt;=$F16,O$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",O$5&gt;=$F16,O$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="P16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",P$5&gt;=$F16,P$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",P$5&gt;=$F16,P$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="Q16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",Q$5&gt;=$F16,Q$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",Q$5&gt;=$F16,Q$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="R16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",R$5&gt;=$F16,R$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",R$5&gt;=$F16,R$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="S16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",S$5&gt;=$F16,S$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",S$5&gt;=$F16,S$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="T16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",T$5&gt;=$F16,T$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",T$5&gt;=$F16,T$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="24"/>
         <v/>
       </c>
       <c r="U16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",U$5&gt;=$F16,U$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",U$5&gt;=$F16,U$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="24"/>
         <v/>
       </c>
       <c r="V16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",V$5&gt;=$F16,V$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",V$5&gt;=$F16,V$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="24"/>
         <v/>
       </c>
       <c r="W16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",W$5&gt;=$F16,W$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",W$5&gt;=$F16,W$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="24"/>
         <v/>
       </c>
       <c r="X16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",X$5&gt;=$F16,X$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",X$5&gt;=$F16,X$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="24"/>
         <v/>
       </c>
       <c r="Y16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",Y$5&gt;=$F16,Y$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",Y$5&gt;=$F16,Y$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="24"/>
         <v/>
       </c>
       <c r="Z16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",Z$5&gt;=$F16,Z$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",Z$5&gt;=$F16,Z$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AA16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",AA$5&gt;=$F16,AA$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",AA$5&gt;=$F16,AA$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AB16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",AB$5&gt;=$F16,AB$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",AB$5&gt;=$F16,AB$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AC16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",AC$5&gt;=$F16,AC$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",AC$5&gt;=$F16,AC$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AD16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",AD$5&gt;=$F16,AD$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",AD$5&gt;=$F16,AD$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AE16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",AE$5&gt;=$F16,AE$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",AE$5&gt;=$F16,AE$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AF16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",AF$5&gt;=$F16,AF$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",AF$5&gt;=$F16,AF$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AG16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",AG$5&gt;=$F16,AG$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",AG$5&gt;=$F16,AG$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AH16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",AH$5&gt;=$F16,AH$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",AH$5&gt;=$F16,AH$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AI16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",AI$5&gt;=$F16,AI$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",AI$5&gt;=$F16,AI$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AJ16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",AJ$5&gt;=$F16,AJ$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",AJ$5&gt;=$F16,AJ$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AK16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",AK$5&gt;=$F16,AK$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",AK$5&gt;=$F16,AK$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AL16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",AL$5&gt;=$F16,AL$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",AL$5&gt;=$F16,AL$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AM16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",AM$5&gt;=$F16,AM$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",AM$5&gt;=$F16,AM$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AN16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",AN$5&gt;=$F16,AN$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",AN$5&gt;=$F16,AN$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AO16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",AO$5&gt;=$F16,AO$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",AO$5&gt;=$F16,AO$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AP16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",AP$5&gt;=$F16,AP$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",AP$5&gt;=$F16,AP$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AQ16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",AQ$5&gt;=$F16,AQ$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",AQ$5&gt;=$F16,AQ$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AR16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",AR$5&gt;=$F16,AR$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",AR$5&gt;=$F16,AR$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AS16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",AS$5&gt;=$F16,AS$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",AS$5&gt;=$F16,AS$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AT16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",AT$5&gt;=$F16,AT$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",AT$5&gt;=$F16,AT$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AU16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",AU$5&gt;=$F16,AU$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",AU$5&gt;=$F16,AU$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AV16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",AV$5&gt;=$F16,AV$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",AV$5&gt;=$F16,AV$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AW16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",AW$5&gt;=$F16,AW$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",AW$5&gt;=$F16,AW$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AX16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",AX$5&gt;=$F16,AX$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",AX$5&gt;=$F16,AX$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AY16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",AY$5&gt;=$F16,AY$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",AY$5&gt;=$F16,AY$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AZ16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",AZ$5&gt;=$F16,AZ$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",AZ$5&gt;=$F16,AZ$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="BA16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",BA$5&gt;=$F16,BA$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",BA$5&gt;=$F16,BA$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="BB16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",BB$5&gt;=$F16,BB$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",BB$5&gt;=$F16,BB$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="BC16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",BC$5&gt;=$F16,BC$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",BC$5&gt;=$F16,BC$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="BD16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",BD$5&gt;=$F16,BD$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",BD$5&gt;=$F16,BD$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="BE16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",BE$5&gt;=$F16,BE$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",BE$5&gt;=$F16,BE$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="BF16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",BF$5&gt;=$F16,BF$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",BF$5&gt;=$F16,BF$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BG16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",BG$5&gt;=$F16,BG$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",BG$5&gt;=$F16,BG$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BH16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",BH$5&gt;=$F16,BH$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",BH$5&gt;=$F16,BH$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BI16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",BI$5&gt;=$F16,BI$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",BI$5&gt;=$F16,BI$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BJ16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",BJ$5&gt;=$F16,BJ$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",BJ$5&gt;=$F16,BJ$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BK16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",BK$5&gt;=$F16,BK$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",BK$5&gt;=$F16,BK$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BL16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",BL$5&gt;=$F16,BL$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",BL$5&gt;=$F16,BL$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BM16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",BM$5&gt;=$F16,BM$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",BM$5&gt;=$F16,BM$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BN16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",BN$5&gt;=$F16,BN$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",BN$5&gt;=$F16,BN$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BO16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",BO$5&gt;=$F16,BO$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",BO$5&gt;=$F16,BO$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BP16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",BP$5&gt;=$F16,BP$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",BP$5&gt;=$F16,BP$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BQ16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",BQ$5&gt;=$F16,BQ$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",BQ$5&gt;=$F16,BQ$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BR16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",BR$5&gt;=$F16,BR$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",BR$5&gt;=$F16,BR$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BS16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",BS$5&gt;=$F16,BS$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",BS$5&gt;=$F16,BS$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BT16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",BT$5&gt;=$F16,BT$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",BT$5&gt;=$F16,BT$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BU16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",BU$5&gt;=$F16,BU$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",BU$5&gt;=$F16,BU$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BV16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",BV$5&gt;=$F16,BV$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",BV$5&gt;=$F16,BV$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BW16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",BW$5&gt;=$F16,BW$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",BW$5&gt;=$F16,BW$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BX16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",BX$5&gt;=$F16,BX$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",BX$5&gt;=$F16,BX$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BY16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",BY$5&gt;=$F16,BY$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",BY$5&gt;=$F16,BY$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BZ16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",BZ$5&gt;=$F16,BZ$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",BZ$5&gt;=$F16,BZ$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="CA16" s="34" t="str">
-        <f ca="1">IF(AND($C16="Goal",CA$5&gt;=$F16,CA$5&lt;=$F16+$H16-1),2,IF(AND($C16="Milestone",CA$5&gt;=$F16,CA$5&lt;=$F16+$H16-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:79" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:79" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="36" t="s">
         <v>48</v>
@@ -5287,7 +5301,7 @@
       <c r="C17" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="60"/>
+      <c r="D17" s="49"/>
       <c r="E17" s="29">
         <v>0</v>
       </c>
@@ -5303,287 +5317,287 @@
       </c>
       <c r="I17" s="25"/>
       <c r="J17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",J$5&gt;=$F17,J$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",J$5&gt;=$F17,J$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="K17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",K$5&gt;=$F17,K$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",K$5&gt;=$F17,K$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="L17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",L$5&gt;=$F17,L$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",L$5&gt;=$F17,L$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="M17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",M$5&gt;=$F17,M$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",M$5&gt;=$F17,M$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="N17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",N$5&gt;=$F17,N$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",N$5&gt;=$F17,N$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="O17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",O$5&gt;=$F17,O$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",O$5&gt;=$F17,O$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="P17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",P$5&gt;=$F17,P$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",P$5&gt;=$F17,P$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="Q17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",Q$5&gt;=$F17,Q$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",Q$5&gt;=$F17,Q$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="R17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",R$5&gt;=$F17,R$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",R$5&gt;=$F17,R$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="S17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",S$5&gt;=$F17,S$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",S$5&gt;=$F17,S$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="T17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",T$5&gt;=$F17,T$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",T$5&gt;=$F17,T$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="24"/>
         <v/>
       </c>
       <c r="U17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",U$5&gt;=$F17,U$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",U$5&gt;=$F17,U$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="24"/>
         <v/>
       </c>
       <c r="V17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",V$5&gt;=$F17,V$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",V$5&gt;=$F17,V$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="24"/>
         <v/>
       </c>
       <c r="W17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",W$5&gt;=$F17,W$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",W$5&gt;=$F17,W$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="24"/>
         <v/>
       </c>
       <c r="X17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",X$5&gt;=$F17,X$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",X$5&gt;=$F17,X$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="24"/>
         <v/>
       </c>
       <c r="Y17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",Y$5&gt;=$F17,Y$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",Y$5&gt;=$F17,Y$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="24"/>
         <v/>
       </c>
       <c r="Z17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",Z$5&gt;=$F17,Z$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",Z$5&gt;=$F17,Z$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AA17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",AA$5&gt;=$F17,AA$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",AA$5&gt;=$F17,AA$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AB17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",AB$5&gt;=$F17,AB$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",AB$5&gt;=$F17,AB$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AC17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",AC$5&gt;=$F17,AC$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",AC$5&gt;=$F17,AC$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AD17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",AD$5&gt;=$F17,AD$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",AD$5&gt;=$F17,AD$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AE17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",AE$5&gt;=$F17,AE$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",AE$5&gt;=$F17,AE$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AF17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",AF$5&gt;=$F17,AF$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",AF$5&gt;=$F17,AF$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AG17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",AG$5&gt;=$F17,AG$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",AG$5&gt;=$F17,AG$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AH17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",AH$5&gt;=$F17,AH$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",AH$5&gt;=$F17,AH$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AI17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",AI$5&gt;=$F17,AI$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",AI$5&gt;=$F17,AI$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AJ17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",AJ$5&gt;=$F17,AJ$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",AJ$5&gt;=$F17,AJ$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AK17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",AK$5&gt;=$F17,AK$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",AK$5&gt;=$F17,AK$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AL17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",AL$5&gt;=$F17,AL$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",AL$5&gt;=$F17,AL$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AM17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",AM$5&gt;=$F17,AM$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",AM$5&gt;=$F17,AM$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AN17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",AN$5&gt;=$F17,AN$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",AN$5&gt;=$F17,AN$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AO17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",AO$5&gt;=$F17,AO$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",AO$5&gt;=$F17,AO$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AP17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",AP$5&gt;=$F17,AP$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",AP$5&gt;=$F17,AP$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AQ17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",AQ$5&gt;=$F17,AQ$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",AQ$5&gt;=$F17,AQ$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AR17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",AR$5&gt;=$F17,AR$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",AR$5&gt;=$F17,AR$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AS17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",AS$5&gt;=$F17,AS$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",AS$5&gt;=$F17,AS$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AT17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",AT$5&gt;=$F17,AT$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",AT$5&gt;=$F17,AT$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AU17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",AU$5&gt;=$F17,AU$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",AU$5&gt;=$F17,AU$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AV17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",AV$5&gt;=$F17,AV$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",AV$5&gt;=$F17,AV$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AW17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",AW$5&gt;=$F17,AW$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",AW$5&gt;=$F17,AW$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AX17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",AX$5&gt;=$F17,AX$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",AX$5&gt;=$F17,AX$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AY17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",AY$5&gt;=$F17,AY$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",AY$5&gt;=$F17,AY$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AZ17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",AZ$5&gt;=$F17,AZ$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",AZ$5&gt;=$F17,AZ$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="BA17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",BA$5&gt;=$F17,BA$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",BA$5&gt;=$F17,BA$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="BB17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",BB$5&gt;=$F17,BB$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",BB$5&gt;=$F17,BB$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="BC17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",BC$5&gt;=$F17,BC$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",BC$5&gt;=$F17,BC$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="BD17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",BD$5&gt;=$F17,BD$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",BD$5&gt;=$F17,BD$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="BE17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",BE$5&gt;=$F17,BE$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",BE$5&gt;=$F17,BE$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="BF17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",BF$5&gt;=$F17,BF$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",BF$5&gt;=$F17,BF$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BG17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",BG$5&gt;=$F17,BG$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",BG$5&gt;=$F17,BG$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BH17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",BH$5&gt;=$F17,BH$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",BH$5&gt;=$F17,BH$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BI17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",BI$5&gt;=$F17,BI$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",BI$5&gt;=$F17,BI$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BJ17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",BJ$5&gt;=$F17,BJ$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",BJ$5&gt;=$F17,BJ$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BK17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",BK$5&gt;=$F17,BK$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",BK$5&gt;=$F17,BK$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BL17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",BL$5&gt;=$F17,BL$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",BL$5&gt;=$F17,BL$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BM17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",BM$5&gt;=$F17,BM$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",BM$5&gt;=$F17,BM$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="BN17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",BN$5&gt;=$F17,BN$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",BN$5&gt;=$F17,BN$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BO17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",BO$5&gt;=$F17,BO$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",BO$5&gt;=$F17,BO$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BP17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",BP$5&gt;=$F17,BP$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",BP$5&gt;=$F17,BP$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BQ17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",BQ$5&gt;=$F17,BQ$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",BQ$5&gt;=$F17,BQ$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BR17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",BR$5&gt;=$F17,BR$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",BR$5&gt;=$F17,BR$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BS17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",BS$5&gt;=$F17,BS$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",BS$5&gt;=$F17,BS$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BT17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",BT$5&gt;=$F17,BT$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",BT$5&gt;=$F17,BT$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BU17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",BU$5&gt;=$F17,BU$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",BU$5&gt;=$F17,BU$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BV17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",BV$5&gt;=$F17,BV$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",BV$5&gt;=$F17,BV$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BW17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",BW$5&gt;=$F17,BW$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",BW$5&gt;=$F17,BW$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BX17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",BX$5&gt;=$F17,BX$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",BX$5&gt;=$F17,BX$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BY17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",BY$5&gt;=$F17,BY$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",BY$5&gt;=$F17,BY$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BZ17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",BZ$5&gt;=$F17,BZ$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",BZ$5&gt;=$F17,BZ$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="CA17" s="34" t="str">
-        <f ca="1">IF(AND($C17="Goal",CA$5&gt;=$F17,CA$5&lt;=$F17+$H17-1),2,IF(AND($C17="Milestone",CA$5&gt;=$F17,CA$5&lt;=$F17+$H17-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:79" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:79" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="15"/>
       <c r="B18" s="37" t="s">
         <v>46</v>
@@ -5876,7 +5890,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:79" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:79" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="36" t="s">
         <v>41</v>
@@ -5884,7 +5898,7 @@
       <c r="C19" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="D19" s="60"/>
+      <c r="D19" s="49"/>
       <c r="E19" s="29">
         <v>0</v>
       </c>
@@ -6180,7 +6194,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:79" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:79" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="B20" s="36" t="s">
         <v>43</v>
@@ -6484,7 +6498,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:79" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:79" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="36" t="s">
         <v>44</v>
@@ -6578,7 +6592,7 @@
       <c r="BZ21" s="34"/>
       <c r="CA21" s="34"/>
     </row>
-    <row r="22" spans="1:79" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:79" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="37" t="s">
         <v>50</v>
@@ -6871,7 +6885,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:79" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:79" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
       <c r="B23" s="36" t="s">
         <v>49</v>
@@ -6879,7 +6893,9 @@
       <c r="C23" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="D23" s="32"/>
+      <c r="D23" s="32" t="s">
+        <v>61</v>
+      </c>
       <c r="E23" s="29">
         <v>0</v>
       </c>
@@ -6965,7 +6981,7 @@
       <c r="BZ23" s="34"/>
       <c r="CA23" s="34"/>
     </row>
-    <row r="24" spans="1:79" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:79" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="14"/>
       <c r="B24" s="37" t="s">
         <v>51</v>
@@ -6978,287 +6994,287 @@
       <c r="H24" s="31"/>
       <c r="I24" s="25"/>
       <c r="J24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",J$5&gt;=$F24,J$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",J$5&gt;=$F24,J$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ref="J24:AO24" ca="1" si="32">IF(AND($C24="Goal",J$5&gt;=$F24,J$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",J$5&gt;=$F24,J$5&lt;=$F24+$H24-1),1,""))</f>
         <v/>
       </c>
       <c r="K24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",K$5&gt;=$F24,K$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",K$5&gt;=$F24,K$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="L24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",L$5&gt;=$F24,L$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",L$5&gt;=$F24,L$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="M24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",M$5&gt;=$F24,M$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",M$5&gt;=$F24,M$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="N24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",N$5&gt;=$F24,N$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",N$5&gt;=$F24,N$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="O24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",O$5&gt;=$F24,O$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",O$5&gt;=$F24,O$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="P24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",P$5&gt;=$F24,P$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",P$5&gt;=$F24,P$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="Q24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",Q$5&gt;=$F24,Q$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",Q$5&gt;=$F24,Q$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="R24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",R$5&gt;=$F24,R$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",R$5&gt;=$F24,R$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="S24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",S$5&gt;=$F24,S$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",S$5&gt;=$F24,S$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="T24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",T$5&gt;=$F24,T$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",T$5&gt;=$F24,T$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="U24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",U$5&gt;=$F24,U$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",U$5&gt;=$F24,U$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="V24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",V$5&gt;=$F24,V$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",V$5&gt;=$F24,V$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="W24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",W$5&gt;=$F24,W$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",W$5&gt;=$F24,W$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="X24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",X$5&gt;=$F24,X$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",X$5&gt;=$F24,X$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="Y24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",Y$5&gt;=$F24,Y$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",Y$5&gt;=$F24,Y$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="Z24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",Z$5&gt;=$F24,Z$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",Z$5&gt;=$F24,Z$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="AA24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",AA$5&gt;=$F24,AA$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",AA$5&gt;=$F24,AA$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="AB24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",AB$5&gt;=$F24,AB$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",AB$5&gt;=$F24,AB$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="AC24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",AC$5&gt;=$F24,AC$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",AC$5&gt;=$F24,AC$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="AD24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",AD$5&gt;=$F24,AD$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",AD$5&gt;=$F24,AD$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="AE24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",AE$5&gt;=$F24,AE$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",AE$5&gt;=$F24,AE$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="AF24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",AF$5&gt;=$F24,AF$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",AF$5&gt;=$F24,AF$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="AG24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",AG$5&gt;=$F24,AG$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",AG$5&gt;=$F24,AG$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="AH24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",AH$5&gt;=$F24,AH$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",AH$5&gt;=$F24,AH$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="AI24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",AI$5&gt;=$F24,AI$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",AI$5&gt;=$F24,AI$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="AJ24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",AJ$5&gt;=$F24,AJ$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",AJ$5&gt;=$F24,AJ$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="AK24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",AK$5&gt;=$F24,AK$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",AK$5&gt;=$F24,AK$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="AL24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",AL$5&gt;=$F24,AL$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",AL$5&gt;=$F24,AL$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="AM24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",AM$5&gt;=$F24,AM$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",AM$5&gt;=$F24,AM$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="AN24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",AN$5&gt;=$F24,AN$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",AN$5&gt;=$F24,AN$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="AO24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",AO$5&gt;=$F24,AO$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",AO$5&gt;=$F24,AO$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="AP24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",AP$5&gt;=$F24,AP$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",AP$5&gt;=$F24,AP$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ref="AP24:BU24" ca="1" si="33">IF(AND($C24="Goal",AP$5&gt;=$F24,AP$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",AP$5&gt;=$F24,AP$5&lt;=$F24+$H24-1),1,""))</f>
         <v/>
       </c>
       <c r="AQ24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",AQ$5&gt;=$F24,AQ$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",AQ$5&gt;=$F24,AQ$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AR24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",AR$5&gt;=$F24,AR$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",AR$5&gt;=$F24,AR$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AS24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",AS$5&gt;=$F24,AS$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",AS$5&gt;=$F24,AS$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AT24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",AT$5&gt;=$F24,AT$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",AT$5&gt;=$F24,AT$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AU24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",AU$5&gt;=$F24,AU$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",AU$5&gt;=$F24,AU$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AV24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",AV$5&gt;=$F24,AV$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",AV$5&gt;=$F24,AV$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AW24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",AW$5&gt;=$F24,AW$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",AW$5&gt;=$F24,AW$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AX24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",AX$5&gt;=$F24,AX$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",AX$5&gt;=$F24,AX$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AY24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",AY$5&gt;=$F24,AY$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",AY$5&gt;=$F24,AY$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AZ24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",AZ$5&gt;=$F24,AZ$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",AZ$5&gt;=$F24,AZ$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BA24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",BA$5&gt;=$F24,BA$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",BA$5&gt;=$F24,BA$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BB24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",BB$5&gt;=$F24,BB$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",BB$5&gt;=$F24,BB$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BC24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",BC$5&gt;=$F24,BC$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",BC$5&gt;=$F24,BC$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BD24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",BD$5&gt;=$F24,BD$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",BD$5&gt;=$F24,BD$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BE24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",BE$5&gt;=$F24,BE$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",BE$5&gt;=$F24,BE$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BF24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",BF$5&gt;=$F24,BF$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",BF$5&gt;=$F24,BF$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BG24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",BG$5&gt;=$F24,BG$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",BG$5&gt;=$F24,BG$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BH24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",BH$5&gt;=$F24,BH$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",BH$5&gt;=$F24,BH$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BI24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",BI$5&gt;=$F24,BI$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",BI$5&gt;=$F24,BI$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BJ24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",BJ$5&gt;=$F24,BJ$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",BJ$5&gt;=$F24,BJ$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BK24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",BK$5&gt;=$F24,BK$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",BK$5&gt;=$F24,BK$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BL24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",BL$5&gt;=$F24,BL$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",BL$5&gt;=$F24,BL$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BM24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",BM$5&gt;=$F24,BM$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",BM$5&gt;=$F24,BM$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BN24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",BN$5&gt;=$F24,BN$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",BN$5&gt;=$F24,BN$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BO24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",BO$5&gt;=$F24,BO$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",BO$5&gt;=$F24,BO$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BP24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",BP$5&gt;=$F24,BP$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",BP$5&gt;=$F24,BP$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BQ24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",BQ$5&gt;=$F24,BQ$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",BQ$5&gt;=$F24,BQ$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BR24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",BR$5&gt;=$F24,BR$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",BR$5&gt;=$F24,BR$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BS24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",BS$5&gt;=$F24,BS$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",BS$5&gt;=$F24,BS$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BT24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",BT$5&gt;=$F24,BT$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",BT$5&gt;=$F24,BT$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BU24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",BU$5&gt;=$F24,BU$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",BU$5&gt;=$F24,BU$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="BV24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",BV$5&gt;=$F24,BV$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",BV$5&gt;=$F24,BV$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ref="BV24:CA24" ca="1" si="34">IF(AND($C24="Goal",BV$5&gt;=$F24,BV$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",BV$5&gt;=$F24,BV$5&lt;=$F24+$H24-1),1,""))</f>
         <v/>
       </c>
       <c r="BW24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",BW$5&gt;=$F24,BW$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",BW$5&gt;=$F24,BW$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="BX24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",BX$5&gt;=$F24,BX$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",BX$5&gt;=$F24,BX$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="BY24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",BY$5&gt;=$F24,BY$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",BY$5&gt;=$F24,BY$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="BZ24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",BZ$5&gt;=$F24,BZ$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",BZ$5&gt;=$F24,BZ$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="CA24" s="34" t="str">
-        <f ca="1">IF(AND($C24="Goal",CA$5&gt;=$F24,CA$5&lt;=$F24+$H24-1),2,IF(AND($C24="Milestone",CA$5&gt;=$F24,CA$5&lt;=$F24+$H24-1),1,""))</f>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:79" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:79" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="14"/>
       <c r="B25" s="36" t="s">
         <v>54</v>
@@ -7266,7 +7282,9 @@
       <c r="C25" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="D25" s="32"/>
+      <c r="D25" s="32" t="s">
+        <v>64</v>
+      </c>
       <c r="E25" s="29">
         <v>0</v>
       </c>
@@ -7352,7 +7370,7 @@
       <c r="BZ25" s="34"/>
       <c r="CA25" s="34"/>
     </row>
-    <row r="26" spans="1:79" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:79" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="14"/>
       <c r="B26" s="36" t="s">
         <v>52</v>
@@ -7446,7 +7464,7 @@
       <c r="BZ26" s="34"/>
       <c r="CA26" s="34"/>
     </row>
-    <row r="27" spans="1:79" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:79" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="14"/>
       <c r="B27" s="36" t="s">
         <v>53</v>
@@ -7540,7 +7558,7 @@
       <c r="BZ27" s="34"/>
       <c r="CA27" s="34"/>
     </row>
-    <row r="28" spans="1:79" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:79" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="14"/>
       <c r="B28" s="36" t="s">
         <v>55</v>
@@ -7634,7 +7652,7 @@
       <c r="BZ28" s="34"/>
       <c r="CA28" s="34"/>
     </row>
-    <row r="29" spans="1:79" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:79" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
       <c r="B29" s="37" t="s">
         <v>31</v>
@@ -7883,51 +7901,51 @@
         <v/>
       </c>
       <c r="BQ29" s="34" t="str">
-        <f t="shared" ref="BQ29:CA34" ca="1" si="30">IF(AND($C29="Goal",BQ$5&gt;=$F29,BQ$5&lt;=$F29+$H29-1),2,IF(AND($C29="Milestone",BQ$5&gt;=$F29,BQ$5&lt;=$F29+$H29-1),1,""))</f>
+        <f t="shared" ref="BQ29:CA34" ca="1" si="35">IF(AND($C29="Goal",BQ$5&gt;=$F29,BQ$5&lt;=$F29+$H29-1),2,IF(AND($C29="Milestone",BQ$5&gt;=$F29,BQ$5&lt;=$F29+$H29-1),1,""))</f>
         <v/>
       </c>
       <c r="BR29" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BS29" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BT29" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BU29" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BV29" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BW29" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BX29" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BY29" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BZ29" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="CA29" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:79" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:79" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="14"/>
       <c r="B30" s="36" t="s">
         <v>45</v>
@@ -8189,51 +8207,51 @@
         <v/>
       </c>
       <c r="BQ30" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BR30" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BS30" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BT30" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BU30" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BV30" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BW30" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BX30" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BY30" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BZ30" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="CA30" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:79" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:79" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="14"/>
       <c r="B31" s="37" t="s">
         <v>32</v>
@@ -8246,287 +8264,287 @@
       <c r="H31" s="31"/>
       <c r="I31" s="25"/>
       <c r="J31" s="34" t="str">
-        <f t="shared" ref="J31:Y34" ca="1" si="31">IF(AND($C31="Goal",J$5&gt;=$F31,J$5&lt;=$F31+$H31-1),2,IF(AND($C31="Milestone",J$5&gt;=$F31,J$5&lt;=$F31+$H31-1),1,""))</f>
+        <f t="shared" ref="J31:Y34" ca="1" si="36">IF(AND($C31="Goal",J$5&gt;=$F31,J$5&lt;=$F31+$H31-1),2,IF(AND($C31="Milestone",J$5&gt;=$F31,J$5&lt;=$F31+$H31-1),1,""))</f>
         <v/>
       </c>
       <c r="K31" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="L31" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="M31" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="N31" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="O31" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="P31" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="Q31" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="R31" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="S31" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="T31" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="U31" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="V31" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="W31" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="X31" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="Y31" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="Z31" s="34" t="str">
-        <f t="shared" ref="Z31:AN34" ca="1" si="32">IF(AND($C31="Goal",Z$5&gt;=$F31,Z$5&lt;=$F31+$H31-1),2,IF(AND($C31="Milestone",Z$5&gt;=$F31,Z$5&lt;=$F31+$H31-1),1,""))</f>
+        <f t="shared" ref="Z31:AN34" ca="1" si="37">IF(AND($C31="Goal",Z$5&gt;=$F31,Z$5&lt;=$F31+$H31-1),2,IF(AND($C31="Milestone",Z$5&gt;=$F31,Z$5&lt;=$F31+$H31-1),1,""))</f>
         <v/>
       </c>
       <c r="AA31" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AB31" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AC31" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AD31" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AE31" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AF31" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AG31" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AH31" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AI31" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AJ31" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AK31" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AL31" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AM31" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AN31" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AO31" s="34" t="str">
-        <f t="shared" ref="AO31:BD34" ca="1" si="33">IF(AND($C31="Goal",AO$5&gt;=$F31,AO$5&lt;=$F31+$H31-1),2,IF(AND($C31="Milestone",AO$5&gt;=$F31,AO$5&lt;=$F31+$H31-1),1,""))</f>
+        <f t="shared" ref="AO31:BD34" ca="1" si="38">IF(AND($C31="Goal",AO$5&gt;=$F31,AO$5&lt;=$F31+$H31-1),2,IF(AND($C31="Milestone",AO$5&gt;=$F31,AO$5&lt;=$F31+$H31-1),1,""))</f>
         <v/>
       </c>
       <c r="AP31" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="AQ31" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="AR31" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="AS31" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="AT31" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="AU31" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="AV31" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="AW31" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="AX31" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="AY31" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="AZ31" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="BA31" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="BB31" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="BC31" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="BD31" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="BE31" s="34" t="str">
-        <f t="shared" ref="BE31:BT34" ca="1" si="34">IF(AND($C31="Goal",BE$5&gt;=$F31,BE$5&lt;=$F31+$H31-1),2,IF(AND($C31="Milestone",BE$5&gt;=$F31,BE$5&lt;=$F31+$H31-1),1,""))</f>
+        <f t="shared" ref="BE31:BT34" ca="1" si="39">IF(AND($C31="Goal",BE$5&gt;=$F31,BE$5&lt;=$F31+$H31-1),2,IF(AND($C31="Milestone",BE$5&gt;=$F31,BE$5&lt;=$F31+$H31-1),1,""))</f>
         <v/>
       </c>
       <c r="BF31" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BG31" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BH31" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BI31" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BJ31" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BK31" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BL31" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BM31" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BN31" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BO31" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BP31" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BQ31" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BR31" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BS31" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BT31" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BU31" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BV31" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BW31" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BX31" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BY31" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BZ31" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="CA31" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:79" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:79" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="14"/>
       <c r="B32" s="36" t="s">
         <v>42</v>
@@ -8552,289 +8570,289 @@
       </c>
       <c r="I32" s="25"/>
       <c r="J32" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="K32" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="L32" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="M32" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="N32" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="O32" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="P32" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="Q32" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="R32" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="S32" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="T32" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="U32" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="V32" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="W32" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="X32" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="Y32" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="Z32" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AA32" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AB32" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AC32" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AD32" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AE32" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AF32" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AG32" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AH32" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AI32" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AJ32" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AK32" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AL32" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AM32" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AN32" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AO32" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="AP32" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="AQ32" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="AR32" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="AS32" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="AT32" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="AU32" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="AV32" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="AW32" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="AX32" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="AY32" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="AZ32" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="BA32" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="BB32" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="BC32" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="BD32" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="BE32" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BF32" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BG32" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BH32" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BI32" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BJ32" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BK32" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BL32" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BM32" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BN32" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BO32" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BP32" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BQ32" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BR32" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BS32" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BT32" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BU32" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BV32" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BW32" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BX32" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BY32" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BZ32" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="CA32" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:79" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:79" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="14"/>
-      <c r="B33" s="59"/>
+      <c r="B33" s="48"/>
       <c r="C33" s="32"/>
       <c r="D33" s="32"/>
       <c r="E33" s="29"/>
@@ -8913,7 +8931,7 @@
       <c r="BZ33" s="34"/>
       <c r="CA33" s="34"/>
     </row>
-    <row r="34" spans="1:79" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:79" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="14" t="s">
         <v>2</v>
       </c>
@@ -8926,388 +8944,387 @@
       <c r="H34" s="31"/>
       <c r="I34" s="25"/>
       <c r="J34" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="K34" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="L34" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="M34" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="N34" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="O34" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="P34" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="Q34" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="R34" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="S34" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="T34" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="U34" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="V34" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="W34" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="X34" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="Y34" s="34" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="Z34" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AA34" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AB34" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AC34" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AD34" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AE34" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AF34" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AG34" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AH34" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AI34" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AJ34" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AK34" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AL34" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AM34" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AN34" s="34" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="AO34" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="AP34" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="AQ34" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="AR34" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="AS34" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="AT34" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="AU34" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="AV34" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="AW34" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="AX34" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="AY34" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="AZ34" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="BA34" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="BB34" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="BC34" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="BD34" s="34" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="38"/>
         <v/>
       </c>
       <c r="BE34" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BF34" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BG34" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BH34" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BI34" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BJ34" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BK34" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BL34" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BM34" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BN34" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BO34" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BP34" s="34" t="str">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
       <c r="BQ34" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BR34" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BS34" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BT34" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BU34" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BV34" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BW34" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BX34" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BY34" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="BZ34" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="CA34" s="34" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:79" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:79" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D35" s="5"/>
       <c r="H35" s="16"/>
       <c r="I35" s="4"/>
     </row>
-    <row r="36" spans="1:79" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:79" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D36" s="6"/>
     </row>
-    <row r="37" spans="1:79" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="1:79" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="1:79" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="1:79" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:79" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:79" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:79" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:79" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:79" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="1:79" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:79" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:79" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="81" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="82" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="85" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="86" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="87" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="88" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="89" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="90" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="91" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="92" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="93" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="94" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="95" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="96" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="97" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="98" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="99" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="100" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="101" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="102" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="103" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="104" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="105" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="106" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="107" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="108" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="109" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="110" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="111" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="112" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="113" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="114" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="115" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="116" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="117" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="118" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="119" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="120" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="121" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="122" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="123" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="124" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="125" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="126" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="127" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:79" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:79" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:79" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:79" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="1:79" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:79" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:79" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:79" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:79" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:79" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:79" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:79" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="52" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="56" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="57" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="59" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="61" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="62" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="63" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="64" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="65" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="66" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="67" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="68" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="69" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="70" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="71" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="72" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="73" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="74" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="75" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="76" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="77" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="78" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="79" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="80" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="81" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="82" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="83" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="84" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="85" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="86" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="87" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="88" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="89" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="90" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="91" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="92" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="93" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="94" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="95" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="96" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="97" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="98" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="99" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="100" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="101" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="102" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="103" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="104" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="105" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="106" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="107" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="108" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="109" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="110" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="111" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="112" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="113" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="114" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="115" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="116" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="117" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="118" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="119" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="120" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="121" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="122" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="123" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="124" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="125" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="126" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="127" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="D3:E3"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="B5:I5"/>
     <mergeCell ref="F3:H3"/>
@@ -9316,6 +9333,7 @@
     <mergeCell ref="X2:AC2"/>
     <mergeCell ref="AE2:AJ2"/>
     <mergeCell ref="AL2:AQ2"/>
+    <mergeCell ref="D3:E3"/>
   </mergeCells>
   <conditionalFormatting sqref="E24:E34 E19 E7:E17">
     <cfRule type="dataBar" priority="89">
@@ -9332,36 +9350,36 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:BZ34">
-    <cfRule type="expression" dxfId="9" priority="82">
+    <cfRule type="expression" dxfId="13" priority="82">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:AN4">
-    <cfRule type="expression" dxfId="8" priority="88">
+    <cfRule type="expression" dxfId="12" priority="88">
       <formula>J$5&lt;=EOMONTH($J$5,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:CA4">
-    <cfRule type="expression" dxfId="7" priority="84">
+    <cfRule type="expression" dxfId="11" priority="84">
       <formula>AND(K$5&lt;=EOMONTH($J$5,2),K$5&gt;EOMONTH($J$5,0),K$5&gt;EOMONTH($J$5,1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:CA4">
-    <cfRule type="expression" dxfId="6" priority="83">
+    <cfRule type="expression" dxfId="10" priority="83">
       <formula>AND(J$5&lt;=EOMONTH($J$5,1),J$5&gt;EOMONTH($J$5,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:CA34">
-    <cfRule type="expression" dxfId="3" priority="105" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="105" stopIfTrue="1">
       <formula>AND($C8="Low",J$5&gt;=$F8,J$5&lt;=$F8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="124" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="124" stopIfTrue="1">
       <formula>AND($C8="High",J$5&gt;=$F8,J$5&lt;=$F8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="142" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="142" stopIfTrue="1">
       <formula>AND($C8="On Track",J$5&gt;=$F8,J$5&lt;=$F8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="143" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="143" stopIfTrue="1">
       <formula>AND($C8="Med",J$5&gt;=$F8,J$5&lt;=$F8+$H8-1)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="5" priority="144" stopIfTrue="1">
@@ -9531,15 +9549,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>25400</xdr:colOff>
+                    <xdr:colOff>23854</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>63500</xdr:rowOff>
+                    <xdr:rowOff>63610</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>84</xdr:col>
-                    <xdr:colOff>127000</xdr:colOff>
+                    <xdr:colOff>127221</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>241300</xdr:rowOff>
+                    <xdr:rowOff>238539</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -9909,33 +9927,33 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="87.1640625" style="10" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="8"/>
+    <col min="1" max="1" width="87.109375" style="10" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="9" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" s="9" customFormat="1" ht="26.3" x14ac:dyDescent="0.5">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="84.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" ht="84.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" ht="26.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="10" customFormat="1" ht="205" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" s="10" customFormat="1" ht="205.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Uodate to presentation and schedule
</commit_message>
<xml_diff>
--- a/Documents/Meeting Updates/Marching Masters Schedule.xlsx
+++ b/Documents/Meeting Updates/Marching Masters Schedule.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA2BB54-B9DE-234B-AA03-354FCC44214D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DFE0B93-3833-154D-B8D8-8554CBDEF742}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20440" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="11" r:id="rId1"/>
@@ -921,16 +921,13 @@
     <xf numFmtId="14" fontId="20" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1">
@@ -952,13 +949,16 @@
     <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="11" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="3"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="20" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -976,23 +976,39 @@
     <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
-  <dxfs count="145">
+  <dxfs count="109">
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
-        <color theme="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1043,697 +1059,6 @@
         </right>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="2" tint="-9.9948118533890809E-2"/>
-        </left>
-        <right style="thin">
-          <color theme="2" tint="-9.9948118533890809E-2"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="7" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="7" tint="-0.24994659260841701"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="6"/>
-        </left>
-        <right style="thin">
-          <color theme="6"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="2" tint="-9.9948118533890809E-2"/>
-        </left>
-        <right style="thin">
-          <color theme="2" tint="-9.9948118533890809E-2"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="7" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="7" tint="-0.24994659260841701"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="6"/>
-        </left>
-        <right style="thin">
-          <color theme="6"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="2" tint="-9.9948118533890809E-2"/>
-        </left>
-        <right style="thin">
-          <color theme="2" tint="-9.9948118533890809E-2"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="7" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="7" tint="-0.24994659260841701"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="6"/>
-        </left>
-        <right style="thin">
-          <color theme="6"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="2" tint="-9.9948118533890809E-2"/>
-        </left>
-        <right style="thin">
-          <color theme="2" tint="-9.9948118533890809E-2"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="7" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="7" tint="-0.24994659260841701"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="6"/>
-        </left>
-        <right style="thin">
-          <color theme="6"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -3503,39 +2828,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <border>
         <left style="thin">
           <color theme="0" tint="-0.24994659260841701"/>
@@ -3680,20 +2972,20 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="Gantt Table Style" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Gantt Table Style" pivot="0" count="3" xr9:uid="{4904D139-63E4-4221-B7C9-C6C5B7A50FAF}">
-      <tableStyleElement type="wholeTable" dxfId="144"/>
-      <tableStyleElement type="headerRow" dxfId="143"/>
-      <tableStyleElement type="firstRowStripe" dxfId="142"/>
+      <tableStyleElement type="wholeTable" dxfId="108"/>
+      <tableStyleElement type="headerRow" dxfId="107"/>
+      <tableStyleElement type="firstRowStripe" dxfId="106"/>
     </tableStyle>
     <tableStyle name="ToDoList" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="141"/>
-      <tableStyleElement type="headerRow" dxfId="140"/>
-      <tableStyleElement type="totalRow" dxfId="139"/>
-      <tableStyleElement type="firstColumn" dxfId="138"/>
-      <tableStyleElement type="lastColumn" dxfId="137"/>
-      <tableStyleElement type="firstRowStripe" dxfId="136"/>
-      <tableStyleElement type="secondRowStripe" dxfId="135"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="134"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="133"/>
+      <tableStyleElement type="wholeTable" dxfId="105"/>
+      <tableStyleElement type="headerRow" dxfId="104"/>
+      <tableStyleElement type="totalRow" dxfId="103"/>
+      <tableStyleElement type="firstColumn" dxfId="102"/>
+      <tableStyleElement type="lastColumn" dxfId="101"/>
+      <tableStyleElement type="firstRowStripe" dxfId="100"/>
+      <tableStyleElement type="secondRowStripe" dxfId="99"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="98"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="97"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -3787,7 +3079,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="39" fmlaLink="$F$4" horiz="1" max="365" page="2" val="14"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="39" fmlaLink="$F$4" horiz="1" max="365" page="2" val="21"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3857,12 +3149,12 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{EE48C34E-B98C-4BBA-90C8-388E8655DD6D}" name="Milestone Description" dataDxfId="132"/>
-    <tableColumn id="2" xr3:uid="{B8ACC97F-C189-49BA-91CF-CB5671185BCF}" name="Category" dataDxfId="131"/>
-    <tableColumn id="3" xr3:uid="{5419FA1B-A035-4F0A-9257-1AA4BCB5E6CF}" name="Assigned To" dataDxfId="130"/>
+    <tableColumn id="1" xr3:uid="{EE48C34E-B98C-4BBA-90C8-388E8655DD6D}" name="Milestone Description" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{B8ACC97F-C189-49BA-91CF-CB5671185BCF}" name="Category" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{5419FA1B-A035-4F0A-9257-1AA4BCB5E6CF}" name="Assigned To" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{A60A6524-18F0-48B7-BB3C-2F4A35799FF7}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{59612C1F-9AAB-483B-A6A5-3563E9D77941}" name="Start" dataCellStyle="Date"/>
-    <tableColumn id="7" xr3:uid="{FFB4566D-F84D-4445-98D2-EC6DB0387316}" name="End" dataDxfId="129" dataCellStyle="Date"/>
+    <tableColumn id="7" xr3:uid="{FFB4566D-F84D-4445-98D2-EC6DB0387316}" name="End" dataDxfId="0" dataCellStyle="Date"/>
     <tableColumn id="6" xr3:uid="{012C59F1-49D4-4A67-B8DD-855C6581FD6A}" name="No. Days" dataCellStyle="Comma [0]"/>
   </tableColumns>
   <tableStyleInfo name="Gantt Table Style" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4142,8 +3434,8 @@
   </sheetPr>
   <dimension ref="A1:CA165"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A20" zoomScaleNormal="150" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A5" zoomScaleNormal="150" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4210,46 +3502,46 @@
       <c r="F2" s="23"/>
       <c r="G2" s="23"/>
       <c r="H2" s="21"/>
-      <c r="J2" s="68" t="s">
+      <c r="J2" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="68"/>
-      <c r="L2" s="68"/>
-      <c r="M2" s="68"/>
-      <c r="N2" s="68"/>
-      <c r="O2" s="68"/>
-      <c r="Q2" s="58" t="s">
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="67"/>
+      <c r="Q2" s="68" t="s">
         <v>51</v>
       </c>
-      <c r="R2" s="58"/>
-      <c r="S2" s="58"/>
-      <c r="T2" s="58"/>
-      <c r="U2" s="58"/>
-      <c r="V2" s="58"/>
-      <c r="X2" s="59" t="s">
+      <c r="R2" s="68"/>
+      <c r="S2" s="68"/>
+      <c r="T2" s="68"/>
+      <c r="U2" s="68"/>
+      <c r="V2" s="68"/>
+      <c r="X2" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="Y2" s="59"/>
-      <c r="Z2" s="59"/>
-      <c r="AA2" s="59"/>
-      <c r="AB2" s="59"/>
-      <c r="AC2" s="59"/>
-      <c r="AE2" s="60" t="s">
+      <c r="Y2" s="69"/>
+      <c r="Z2" s="69"/>
+      <c r="AA2" s="69"/>
+      <c r="AB2" s="69"/>
+      <c r="AC2" s="69"/>
+      <c r="AE2" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="AF2" s="60"/>
-      <c r="AG2" s="60"/>
-      <c r="AH2" s="60"/>
-      <c r="AI2" s="60"/>
-      <c r="AJ2" s="60"/>
-      <c r="AL2" s="61" t="s">
+      <c r="AF2" s="70"/>
+      <c r="AG2" s="70"/>
+      <c r="AH2" s="70"/>
+      <c r="AI2" s="70"/>
+      <c r="AJ2" s="70"/>
+      <c r="AL2" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="AM2" s="61"/>
-      <c r="AN2" s="61"/>
-      <c r="AO2" s="61"/>
-      <c r="AP2" s="61"/>
-      <c r="AQ2" s="61"/>
+      <c r="AM2" s="71"/>
+      <c r="AN2" s="71"/>
+      <c r="AO2" s="71"/>
+      <c r="AP2" s="71"/>
+      <c r="AQ2" s="71"/>
       <c r="AR2" s="20"/>
       <c r="AW2" s="20"/>
       <c r="BB2" s="20"/>
@@ -4260,28 +3552,28 @@
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
-      <c r="D3" s="62" t="s">
+      <c r="D3" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="63"/>
-      <c r="F3" s="65">
+      <c r="E3" s="62"/>
+      <c r="F3" s="64">
         <f ca="1">IFERROR(IF(MIN(Milestones[Start])=0,TODAY(),MIN(Milestones[Start])),TODAY())</f>
         <v>44096</v>
       </c>
-      <c r="G3" s="66"/>
-      <c r="H3" s="67"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="66"/>
       <c r="I3" s="22"/>
     </row>
     <row r="4" spans="1:79" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="62" t="s">
+      <c r="D4" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="63"/>
+      <c r="E4" s="62"/>
       <c r="F4" s="39">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="G4" s="47"/>
       <c r="J4" s="38" t="str">
@@ -4316,7 +3608,7 @@
       <c r="AD4" s="38"/>
       <c r="AE4" s="38" t="str">
         <f ca="1">IF(OR(TEXT(AE5,"mmmm")=X4,TEXT(AE5,"mmmm")=Q4,TEXT(AE5,"mmmm")=J4),"",TEXT(AE5,"mmmm"))</f>
-        <v/>
+        <v>November</v>
       </c>
       <c r="AF4" s="38"/>
       <c r="AG4" s="38"/>
@@ -4326,7 +3618,7 @@
       <c r="AK4" s="38"/>
       <c r="AL4" s="38" t="str">
         <f ca="1">IF(OR(TEXT(AL5,"mmmm")=AE4,TEXT(AL5,"mmmm")=X4,TEXT(AL5,"mmmm")=Q4,TEXT(AL5,"mmmm")=J4),"",TEXT(AL5,"mmmm"))</f>
-        <v>November</v>
+        <v/>
       </c>
       <c r="AM4" s="38"/>
       <c r="AN4" s="38"/>
@@ -4356,7 +3648,7 @@
       <c r="BF4" s="38"/>
       <c r="BG4" s="38" t="str">
         <f ca="1">IF(OR(TEXT(BG5,"mmmm")=AZ4,TEXT(BG5,"mmmm")=AS4,TEXT(BG5,"mmmm")=AL4,TEXT(BG5,"mmmm")=AE4),"",TEXT(BG5,"mmmm"))</f>
-        <v/>
+        <v>December</v>
       </c>
       <c r="BH4" s="38"/>
       <c r="BI4" s="38"/>
@@ -4383,293 +3675,293 @@
       <c r="A5" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="64"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64"/>
-      <c r="G5" s="64"/>
-      <c r="H5" s="64"/>
-      <c r="I5" s="64"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="63"/>
       <c r="J5" s="43">
         <f ca="1">IFERROR(Project_Start+Scrolling_Increment,TODAY())</f>
-        <v>44110</v>
+        <v>44117</v>
       </c>
       <c r="K5" s="44">
         <f ca="1">J5+1</f>
-        <v>44111</v>
+        <v>44118</v>
       </c>
       <c r="L5" s="44">
         <f t="shared" ref="L5:AY5" ca="1" si="0">K5+1</f>
-        <v>44112</v>
+        <v>44119</v>
       </c>
       <c r="M5" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>44113</v>
+        <v>44120</v>
       </c>
       <c r="N5" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>44114</v>
+        <v>44121</v>
       </c>
       <c r="O5" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>44115</v>
+        <v>44122</v>
       </c>
       <c r="P5" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>44116</v>
+        <v>44123</v>
       </c>
       <c r="Q5" s="43">
         <f ca="1">P5+1</f>
-        <v>44117</v>
+        <v>44124</v>
       </c>
       <c r="R5" s="44">
         <f ca="1">Q5+1</f>
-        <v>44118</v>
+        <v>44125</v>
       </c>
       <c r="S5" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>44119</v>
+        <v>44126</v>
       </c>
       <c r="T5" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>44120</v>
+        <v>44127</v>
       </c>
       <c r="U5" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>44121</v>
+        <v>44128</v>
       </c>
       <c r="V5" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>44122</v>
+        <v>44129</v>
       </c>
       <c r="W5" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>44123</v>
+        <v>44130</v>
       </c>
       <c r="X5" s="43">
         <f ca="1">W5+1</f>
-        <v>44124</v>
+        <v>44131</v>
       </c>
       <c r="Y5" s="44">
         <f ca="1">X5+1</f>
-        <v>44125</v>
+        <v>44132</v>
       </c>
       <c r="Z5" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>44126</v>
+        <v>44133</v>
       </c>
       <c r="AA5" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>44127</v>
+        <v>44134</v>
       </c>
       <c r="AB5" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>44128</v>
+        <v>44135</v>
       </c>
       <c r="AC5" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>44129</v>
+        <v>44136</v>
       </c>
       <c r="AD5" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>44130</v>
+        <v>44137</v>
       </c>
       <c r="AE5" s="43">
         <f ca="1">AD5+1</f>
-        <v>44131</v>
+        <v>44138</v>
       </c>
       <c r="AF5" s="44">
         <f ca="1">AE5+1</f>
-        <v>44132</v>
+        <v>44139</v>
       </c>
       <c r="AG5" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>44133</v>
+        <v>44140</v>
       </c>
       <c r="AH5" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>44134</v>
+        <v>44141</v>
       </c>
       <c r="AI5" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>44135</v>
+        <v>44142</v>
       </c>
       <c r="AJ5" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>44136</v>
+        <v>44143</v>
       </c>
       <c r="AK5" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>44137</v>
+        <v>44144</v>
       </c>
       <c r="AL5" s="43">
         <f ca="1">AK5+1</f>
-        <v>44138</v>
+        <v>44145</v>
       </c>
       <c r="AM5" s="44">
         <f ca="1">AL5+1</f>
-        <v>44139</v>
+        <v>44146</v>
       </c>
       <c r="AN5" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>44140</v>
+        <v>44147</v>
       </c>
       <c r="AO5" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>44141</v>
+        <v>44148</v>
       </c>
       <c r="AP5" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>44142</v>
+        <v>44149</v>
       </c>
       <c r="AQ5" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>44143</v>
+        <v>44150</v>
       </c>
       <c r="AR5" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>44144</v>
+        <v>44151</v>
       </c>
       <c r="AS5" s="43">
         <f ca="1">AR5+1</f>
-        <v>44145</v>
+        <v>44152</v>
       </c>
       <c r="AT5" s="44">
         <f ca="1">AS5+1</f>
-        <v>44146</v>
+        <v>44153</v>
       </c>
       <c r="AU5" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>44147</v>
+        <v>44154</v>
       </c>
       <c r="AV5" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>44148</v>
+        <v>44155</v>
       </c>
       <c r="AW5" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>44149</v>
+        <v>44156</v>
       </c>
       <c r="AX5" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>44150</v>
+        <v>44157</v>
       </c>
       <c r="AY5" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>44151</v>
+        <v>44158</v>
       </c>
       <c r="AZ5" s="43">
         <f ca="1">AY5+1</f>
-        <v>44152</v>
+        <v>44159</v>
       </c>
       <c r="BA5" s="44">
         <f ca="1">AZ5+1</f>
-        <v>44153</v>
+        <v>44160</v>
       </c>
       <c r="BB5" s="44">
         <f t="shared" ref="BB5:BF5" ca="1" si="1">BA5+1</f>
-        <v>44154</v>
+        <v>44161</v>
       </c>
       <c r="BC5" s="44">
         <f t="shared" ca="1" si="1"/>
-        <v>44155</v>
+        <v>44162</v>
       </c>
       <c r="BD5" s="44">
         <f t="shared" ca="1" si="1"/>
-        <v>44156</v>
+        <v>44163</v>
       </c>
       <c r="BE5" s="44">
         <f t="shared" ca="1" si="1"/>
-        <v>44157</v>
+        <v>44164</v>
       </c>
       <c r="BF5" s="45">
         <f t="shared" ca="1" si="1"/>
-        <v>44158</v>
+        <v>44165</v>
       </c>
       <c r="BG5" s="43">
         <f ca="1">BF5+1</f>
-        <v>44159</v>
+        <v>44166</v>
       </c>
       <c r="BH5" s="44">
         <f ca="1">BG5+1</f>
-        <v>44160</v>
+        <v>44167</v>
       </c>
       <c r="BI5" s="44">
         <f t="shared" ref="BI5:BM5" ca="1" si="2">BH5+1</f>
-        <v>44161</v>
+        <v>44168</v>
       </c>
       <c r="BJ5" s="44">
         <f t="shared" ca="1" si="2"/>
-        <v>44162</v>
+        <v>44169</v>
       </c>
       <c r="BK5" s="44">
         <f t="shared" ca="1" si="2"/>
-        <v>44163</v>
+        <v>44170</v>
       </c>
       <c r="BL5" s="44">
         <f t="shared" ca="1" si="2"/>
-        <v>44164</v>
+        <v>44171</v>
       </c>
       <c r="BM5" s="45">
         <f t="shared" ca="1" si="2"/>
-        <v>44165</v>
+        <v>44172</v>
       </c>
       <c r="BN5" s="45">
         <f t="shared" ref="BN5" ca="1" si="3">BM5+1</f>
-        <v>44166</v>
+        <v>44173</v>
       </c>
       <c r="BO5" s="45">
         <f t="shared" ref="BO5" ca="1" si="4">BN5+1</f>
-        <v>44167</v>
+        <v>44174</v>
       </c>
       <c r="BP5" s="45">
         <f t="shared" ref="BP5" ca="1" si="5">BO5+1</f>
-        <v>44168</v>
+        <v>44175</v>
       </c>
       <c r="BQ5" s="45">
         <f t="shared" ref="BQ5" ca="1" si="6">BP5+1</f>
-        <v>44169</v>
+        <v>44176</v>
       </c>
       <c r="BR5" s="45">
         <f t="shared" ref="BR5" ca="1" si="7">BQ5+1</f>
-        <v>44170</v>
+        <v>44177</v>
       </c>
       <c r="BS5" s="45">
         <f t="shared" ref="BS5" ca="1" si="8">BR5+1</f>
-        <v>44171</v>
+        <v>44178</v>
       </c>
       <c r="BT5" s="45">
         <f t="shared" ref="BT5" ca="1" si="9">BS5+1</f>
-        <v>44172</v>
+        <v>44179</v>
       </c>
       <c r="BU5" s="45">
         <f t="shared" ref="BU5" ca="1" si="10">BT5+1</f>
-        <v>44173</v>
+        <v>44180</v>
       </c>
       <c r="BV5" s="45">
         <f t="shared" ref="BV5" ca="1" si="11">BU5+1</f>
-        <v>44174</v>
+        <v>44181</v>
       </c>
       <c r="BW5" s="45">
         <f t="shared" ref="BW5" ca="1" si="12">BV5+1</f>
-        <v>44175</v>
+        <v>44182</v>
       </c>
       <c r="BX5" s="45">
         <f t="shared" ref="BX5" ca="1" si="13">BW5+1</f>
-        <v>44176</v>
+        <v>44183</v>
       </c>
       <c r="BY5" s="45">
         <f t="shared" ref="BY5" ca="1" si="14">BX5+1</f>
-        <v>44177</v>
+        <v>44184</v>
       </c>
       <c r="BZ5" s="45">
         <f t="shared" ref="BZ5" ca="1" si="15">BY5+1</f>
-        <v>44178</v>
+        <v>44185</v>
       </c>
       <c r="CA5" s="45">
         <f t="shared" ref="CA5" ca="1" si="16">BZ5+1</f>
-        <v>44179</v>
+        <v>44186</v>
       </c>
     </row>
     <row r="6" spans="1:79" s="20" customFormat="1" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -14911,33 +14203,33 @@
         <f t="shared" ca="1" si="66"/>
         <v/>
       </c>
-      <c r="AM66" s="34" t="str">
+      <c r="AM66" s="34">
         <f t="shared" ca="1" si="66"/>
-        <v/>
-      </c>
-      <c r="AN66" s="34" t="str">
+        <v>2</v>
+      </c>
+      <c r="AN66" s="34">
         <f t="shared" ref="AN66:AW72" ca="1" si="67">IF(AND($C66="Goal",AN$5&gt;=$F66,AN$5&lt;=$F66+$H66-1),2,IF(AND($C66="Milestone",AN$5&gt;=$F66,AN$5&lt;=$F66+$H66-1),1,""))</f>
-        <v/>
-      </c>
-      <c r="AO66" s="34" t="str">
+        <v>2</v>
+      </c>
+      <c r="AO66" s="34">
         <f t="shared" ca="1" si="67"/>
-        <v/>
-      </c>
-      <c r="AP66" s="34" t="str">
+        <v>2</v>
+      </c>
+      <c r="AP66" s="34">
         <f t="shared" ca="1" si="67"/>
-        <v/>
-      </c>
-      <c r="AQ66" s="34" t="str">
+        <v>2</v>
+      </c>
+      <c r="AQ66" s="34">
         <f t="shared" ca="1" si="67"/>
-        <v/>
-      </c>
-      <c r="AR66" s="34" t="str">
+        <v>2</v>
+      </c>
+      <c r="AR66" s="34">
         <f t="shared" ca="1" si="67"/>
-        <v/>
-      </c>
-      <c r="AS66" s="34" t="str">
+        <v>2</v>
+      </c>
+      <c r="AS66" s="34">
         <f t="shared" ca="1" si="67"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="AT66" s="34">
         <f t="shared" ca="1" si="67"/>
@@ -14995,33 +14287,33 @@
         <f t="shared" ca="1" si="68"/>
         <v>2</v>
       </c>
-      <c r="BH66" s="34">
+      <c r="BH66" s="34" t="str">
         <f t="shared" ref="BH66:BQ72" ca="1" si="69">IF(AND($C66="Goal",BH$5&gt;=$F66,BH$5&lt;=$F66+$H66-1),2,IF(AND($C66="Milestone",BH$5&gt;=$F66,BH$5&lt;=$F66+$H66-1),1,""))</f>
-        <v>2</v>
-      </c>
-      <c r="BI66" s="34">
+        <v/>
+      </c>
+      <c r="BI66" s="34" t="str">
         <f t="shared" ca="1" si="69"/>
-        <v>2</v>
-      </c>
-      <c r="BJ66" s="34">
+        <v/>
+      </c>
+      <c r="BJ66" s="34" t="str">
         <f t="shared" ca="1" si="69"/>
-        <v>2</v>
-      </c>
-      <c r="BK66" s="34">
+        <v/>
+      </c>
+      <c r="BK66" s="34" t="str">
         <f t="shared" ca="1" si="69"/>
-        <v>2</v>
-      </c>
-      <c r="BL66" s="34">
+        <v/>
+      </c>
+      <c r="BL66" s="34" t="str">
         <f t="shared" ca="1" si="69"/>
-        <v>2</v>
-      </c>
-      <c r="BM66" s="34">
+        <v/>
+      </c>
+      <c r="BM66" s="34" t="str">
         <f t="shared" ca="1" si="69"/>
-        <v>2</v>
-      </c>
-      <c r="BN66" s="34">
+        <v/>
+      </c>
+      <c r="BN66" s="34" t="str">
         <f t="shared" ca="1" si="69"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="BO66" s="34" t="str">
         <f t="shared" ca="1" si="69"/>
@@ -16116,33 +15408,33 @@
         <f t="shared" ca="1" si="66"/>
         <v/>
       </c>
-      <c r="AM70" s="34" t="str">
+      <c r="AM70" s="34">
         <f t="shared" ca="1" si="66"/>
-        <v/>
-      </c>
-      <c r="AN70" s="34" t="str">
+        <v>2</v>
+      </c>
+      <c r="AN70" s="34">
         <f t="shared" ca="1" si="67"/>
-        <v/>
-      </c>
-      <c r="AO70" s="34" t="str">
+        <v>2</v>
+      </c>
+      <c r="AO70" s="34">
         <f t="shared" ca="1" si="67"/>
-        <v/>
-      </c>
-      <c r="AP70" s="34" t="str">
+        <v>2</v>
+      </c>
+      <c r="AP70" s="34">
         <f t="shared" ca="1" si="67"/>
-        <v/>
-      </c>
-      <c r="AQ70" s="34" t="str">
+        <v>2</v>
+      </c>
+      <c r="AQ70" s="34">
         <f t="shared" ca="1" si="67"/>
-        <v/>
-      </c>
-      <c r="AR70" s="34" t="str">
+        <v>2</v>
+      </c>
+      <c r="AR70" s="34">
         <f t="shared" ca="1" si="67"/>
-        <v/>
-      </c>
-      <c r="AS70" s="34" t="str">
+        <v>2</v>
+      </c>
+      <c r="AS70" s="34">
         <f t="shared" ca="1" si="67"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="AT70" s="34">
         <f t="shared" ca="1" si="67"/>
@@ -16200,33 +15492,33 @@
         <f t="shared" ca="1" si="68"/>
         <v>2</v>
       </c>
-      <c r="BH70" s="34">
+      <c r="BH70" s="34" t="str">
         <f t="shared" ca="1" si="69"/>
-        <v>2</v>
-      </c>
-      <c r="BI70" s="34">
+        <v/>
+      </c>
+      <c r="BI70" s="34" t="str">
         <f t="shared" ca="1" si="69"/>
-        <v>2</v>
-      </c>
-      <c r="BJ70" s="34">
+        <v/>
+      </c>
+      <c r="BJ70" s="34" t="str">
         <f t="shared" ca="1" si="69"/>
-        <v>2</v>
-      </c>
-      <c r="BK70" s="34">
+        <v/>
+      </c>
+      <c r="BK70" s="34" t="str">
         <f t="shared" ca="1" si="69"/>
-        <v>2</v>
-      </c>
-      <c r="BL70" s="34">
+        <v/>
+      </c>
+      <c r="BL70" s="34" t="str">
         <f t="shared" ca="1" si="69"/>
-        <v>2</v>
-      </c>
-      <c r="BM70" s="34">
+        <v/>
+      </c>
+      <c r="BM70" s="34" t="str">
         <f t="shared" ca="1" si="69"/>
-        <v>2</v>
-      </c>
-      <c r="BN70" s="34">
+        <v/>
+      </c>
+      <c r="BN70" s="34" t="str">
         <f t="shared" ca="1" si="69"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="BO70" s="34" t="str">
         <f t="shared" ca="1" si="69"/>
@@ -16283,11 +15575,11 @@
     </row>
     <row r="71" spans="1:79" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="14"/>
-      <c r="B71" s="70"/>
+      <c r="B71" s="59"/>
       <c r="C71" s="54"/>
       <c r="D71" s="54"/>
-      <c r="E71" s="69"/>
-      <c r="F71" s="71"/>
+      <c r="E71" s="58"/>
+      <c r="F71" s="60"/>
       <c r="G71" s="30"/>
       <c r="H71" s="31"/>
       <c r="I71" s="25"/>
@@ -16966,15 +16258,15 @@
     <row r="165" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="X2:AC2"/>
+    <mergeCell ref="AE2:AJ2"/>
+    <mergeCell ref="AL2:AQ2"/>
+    <mergeCell ref="D3:E3"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="B5:I5"/>
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="J2:O2"/>
     <mergeCell ref="Q2:V2"/>
-    <mergeCell ref="X2:AC2"/>
-    <mergeCell ref="AE2:AJ2"/>
-    <mergeCell ref="AL2:AQ2"/>
-    <mergeCell ref="D3:E3"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:E11 E16 E13:E14 E53 E23:E24 E64:E65 E72 E33 E69">
     <cfRule type="dataBar" priority="339">
@@ -16991,39 +16283,39 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:BZ11 J13:BZ16 J53:BZ53 J44:BZ44 J23:BZ24 J64:BZ65 J26:BZ33">
-    <cfRule type="expression" dxfId="128" priority="332">
+    <cfRule type="expression" dxfId="96" priority="332">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:AN4">
-    <cfRule type="expression" dxfId="127" priority="338">
+    <cfRule type="expression" dxfId="95" priority="338">
       <formula>J$5&lt;=EOMONTH($J$5,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:CA4">
-    <cfRule type="expression" dxfId="126" priority="334">
+    <cfRule type="expression" dxfId="94" priority="334">
       <formula>AND(K$5&lt;=EOMONTH($J$5,2),K$5&gt;EOMONTH($J$5,0),K$5&gt;EOMONTH($J$5,1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:CA4">
-    <cfRule type="expression" dxfId="125" priority="333">
+    <cfRule type="expression" dxfId="93" priority="333">
       <formula>AND(J$5&lt;=EOMONTH($J$5,1),J$5&gt;EOMONTH($J$5,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:CA11 J26:CA33 J38:CA39 J44:CA44 J50:CA51 J53:CA53 J56:CA56 J64:CA65 J13:CA24">
-    <cfRule type="expression" dxfId="124" priority="355" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="355" stopIfTrue="1">
       <formula>AND($C8="Low",J$5&gt;=$F8,J$5&lt;=$F8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="123" priority="374" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="374" stopIfTrue="1">
       <formula>AND($C8="High",J$5&gt;=$F8,J$5&lt;=$F8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="122" priority="392" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="392" stopIfTrue="1">
       <formula>AND($C8="On Track",J$5&gt;=$F8,J$5&lt;=$F8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="121" priority="393" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="393" stopIfTrue="1">
       <formula>AND($C8="Med",J$5&gt;=$F8,J$5&lt;=$F8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="120" priority="394" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="394" stopIfTrue="1">
       <formula>AND(LEN($C8)=0,J$5&gt;=$F8,J$5&lt;=$F8+$H8-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17070,7 +16362,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CA5:CA11 CA13:CA16 CA53 CA44 CA23:CA24 CA64:CA65 CA33">
-    <cfRule type="expression" dxfId="119" priority="453">
+    <cfRule type="expression" dxfId="87" priority="453">
       <formula>AND(TODAY()&gt;=CA$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17089,12 +16381,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J17:BZ18">
-    <cfRule type="expression" dxfId="118" priority="242">
+    <cfRule type="expression" dxfId="86" priority="242">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CA17:CA18 CA26:CA32">
-    <cfRule type="expression" dxfId="117" priority="249">
+    <cfRule type="expression" dxfId="85" priority="249">
       <formula>AND(TODAY()&gt;=CA$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17113,12 +16405,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J19:BZ22">
-    <cfRule type="expression" dxfId="116" priority="233">
+    <cfRule type="expression" dxfId="84" priority="233">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CA19:CA22">
-    <cfRule type="expression" dxfId="115" priority="240">
+    <cfRule type="expression" dxfId="83" priority="240">
       <formula>AND(TODAY()&gt;=CA$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17151,29 +16443,29 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:BZ12">
-    <cfRule type="expression" dxfId="114" priority="223">
+    <cfRule type="expression" dxfId="82" priority="223">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:CA12">
-    <cfRule type="expression" dxfId="113" priority="225" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="225" stopIfTrue="1">
       <formula>AND($C12="Low",J$5&gt;=$F12,J$5&lt;=$F12+$H12-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="226" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="226" stopIfTrue="1">
       <formula>AND($C12="High",J$5&gt;=$F12,J$5&lt;=$F12+$H12-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="111" priority="227" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="227" stopIfTrue="1">
       <formula>AND($C12="On Track",J$5&gt;=$F12,J$5&lt;=$F12+$H12-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="110" priority="228" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="228" stopIfTrue="1">
       <formula>AND($C12="Med",J$5&gt;=$F12,J$5&lt;=$F12+$H12-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="229" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="229" stopIfTrue="1">
       <formula>AND(LEN($C12)=0,J$5&gt;=$F12,J$5&lt;=$F12+$H12-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CA12">
-    <cfRule type="expression" dxfId="108" priority="230">
+    <cfRule type="expression" dxfId="76" priority="230">
       <formula>AND(TODAY()&gt;=CA$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17192,12 +16484,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J38:BZ38">
-    <cfRule type="expression" dxfId="107" priority="214">
+    <cfRule type="expression" dxfId="75" priority="214">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CA38">
-    <cfRule type="expression" dxfId="106" priority="220">
+    <cfRule type="expression" dxfId="74" priority="220">
       <formula>AND(TODAY()&gt;=CA$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17216,12 +16508,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J50:BZ50 J53:BZ53">
-    <cfRule type="expression" dxfId="105" priority="205">
+    <cfRule type="expression" dxfId="73" priority="205">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CA50 CA53">
-    <cfRule type="expression" dxfId="104" priority="211">
+    <cfRule type="expression" dxfId="72" priority="211">
       <formula>AND(TODAY()&gt;=CA$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17240,22 +16532,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J39:BZ39">
-    <cfRule type="expression" dxfId="103" priority="194">
+    <cfRule type="expression" dxfId="71" priority="194">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CA39">
-    <cfRule type="expression" dxfId="102" priority="200">
+    <cfRule type="expression" dxfId="70" priority="200">
       <formula>AND(TODAY()&gt;=CA$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J56:BZ56">
-    <cfRule type="expression" dxfId="101" priority="185">
+    <cfRule type="expression" dxfId="69" priority="185">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CA56">
-    <cfRule type="expression" dxfId="100" priority="186">
+    <cfRule type="expression" dxfId="68" priority="186">
       <formula>AND(TODAY()&gt;=CA$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17288,22 +16580,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J51:BZ51">
-    <cfRule type="expression" dxfId="99" priority="175">
+    <cfRule type="expression" dxfId="67" priority="175">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CA51">
-    <cfRule type="expression" dxfId="98" priority="182">
+    <cfRule type="expression" dxfId="66" priority="182">
       <formula>AND(TODAY()&gt;=CA$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J51:BZ51">
-    <cfRule type="expression" dxfId="97" priority="173">
+    <cfRule type="expression" dxfId="65" priority="173">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CA51">
-    <cfRule type="expression" dxfId="96" priority="174">
+    <cfRule type="expression" dxfId="64" priority="174">
       <formula>AND(TODAY()&gt;=CA$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17364,238 +16656,238 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J25:BZ25">
-    <cfRule type="expression" dxfId="95" priority="131">
+    <cfRule type="expression" dxfId="63" priority="131">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J25:CA25">
-    <cfRule type="expression" dxfId="94" priority="134" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="134" stopIfTrue="1">
       <formula>AND($C25="Low",J$5&gt;=$F25,J$5&lt;=$F25+$H25-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="93" priority="135" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="135" stopIfTrue="1">
       <formula>AND($C25="High",J$5&gt;=$F25,J$5&lt;=$F25+$H25-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="92" priority="136" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="136" stopIfTrue="1">
       <formula>AND($C25="On Track",J$5&gt;=$F25,J$5&lt;=$F25+$H25-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="137" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="137" stopIfTrue="1">
       <formula>AND($C25="Med",J$5&gt;=$F25,J$5&lt;=$F25+$H25-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="138" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="138" stopIfTrue="1">
       <formula>AND(LEN($C25)=0,J$5&gt;=$F25,J$5&lt;=$F25+$H25-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CA25">
-    <cfRule type="expression" dxfId="89" priority="132">
+    <cfRule type="expression" dxfId="57" priority="132">
       <formula>AND(TODAY()&gt;=CA$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J34:BZ37">
-    <cfRule type="expression" dxfId="88" priority="108">
+    <cfRule type="expression" dxfId="56" priority="108">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J34:CA37">
-    <cfRule type="expression" dxfId="87" priority="109" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="109" stopIfTrue="1">
       <formula>AND($C34="Low",J$5&gt;=$F34,J$5&lt;=$F34+$H34-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="110" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="110" stopIfTrue="1">
       <formula>AND($C34="High",J$5&gt;=$F34,J$5&lt;=$F34+$H34-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="85" priority="111" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="111" stopIfTrue="1">
       <formula>AND($C34="On Track",J$5&gt;=$F34,J$5&lt;=$F34+$H34-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="112" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="112" stopIfTrue="1">
       <formula>AND($C34="Med",J$5&gt;=$F34,J$5&lt;=$F34+$H34-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="113" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="113" stopIfTrue="1">
       <formula>AND(LEN($C34)=0,J$5&gt;=$F34,J$5&lt;=$F34+$H34-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CA34:CA37">
-    <cfRule type="expression" dxfId="82" priority="107">
+    <cfRule type="expression" dxfId="50" priority="107">
       <formula>AND(TODAY()&gt;=CA$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J40:BZ43">
-    <cfRule type="expression" dxfId="81" priority="100">
+    <cfRule type="expression" dxfId="49" priority="100">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J40:CA43">
-    <cfRule type="expression" dxfId="80" priority="101" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="101" stopIfTrue="1">
       <formula>AND($C40="Low",J$5&gt;=$F40,J$5&lt;=$F40+$H40-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="102" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="102" stopIfTrue="1">
       <formula>AND($C40="High",J$5&gt;=$F40,J$5&lt;=$F40+$H40-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="103" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="103" stopIfTrue="1">
       <formula>AND($C40="On Track",J$5&gt;=$F40,J$5&lt;=$F40+$H40-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="104" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="104" stopIfTrue="1">
       <formula>AND($C40="Med",J$5&gt;=$F40,J$5&lt;=$F40+$H40-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="105" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="105" stopIfTrue="1">
       <formula>AND(LEN($C40)=0,J$5&gt;=$F40,J$5&lt;=$F40+$H40-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CA40:CA43">
-    <cfRule type="expression" dxfId="75" priority="99">
+    <cfRule type="expression" dxfId="43" priority="99">
       <formula>AND(TODAY()&gt;=CA$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J45:BZ49">
-    <cfRule type="expression" dxfId="74" priority="92">
+    <cfRule type="expression" dxfId="42" priority="92">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J45:CA49">
-    <cfRule type="expression" dxfId="73" priority="93" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="93" stopIfTrue="1">
       <formula>AND($C45="Low",J$5&gt;=$F45,J$5&lt;=$F45+$H45-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="94" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="94" stopIfTrue="1">
       <formula>AND($C45="High",J$5&gt;=$F45,J$5&lt;=$F45+$H45-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="95" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="95" stopIfTrue="1">
       <formula>AND($C45="On Track",J$5&gt;=$F45,J$5&lt;=$F45+$H45-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="96" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="96" stopIfTrue="1">
       <formula>AND($C45="Med",J$5&gt;=$F45,J$5&lt;=$F45+$H45-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="97" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="97" stopIfTrue="1">
       <formula>AND(LEN($C45)=0,J$5&gt;=$F45,J$5&lt;=$F45+$H45-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CA45:CA49">
-    <cfRule type="expression" dxfId="68" priority="91">
+    <cfRule type="expression" dxfId="36" priority="91">
       <formula>AND(TODAY()&gt;=CA$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J52:BZ52">
-    <cfRule type="expression" dxfId="67" priority="84">
+    <cfRule type="expression" dxfId="35" priority="84">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J52:CA52">
-    <cfRule type="expression" dxfId="66" priority="85" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="85" stopIfTrue="1">
       <formula>AND($C52="Low",J$5&gt;=$F52,J$5&lt;=$F52+$H52-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="86" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="86" stopIfTrue="1">
       <formula>AND($C52="High",J$5&gt;=$F52,J$5&lt;=$F52+$H52-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="87" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="87" stopIfTrue="1">
       <formula>AND($C52="On Track",J$5&gt;=$F52,J$5&lt;=$F52+$H52-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="88" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="88" stopIfTrue="1">
       <formula>AND($C52="Med",J$5&gt;=$F52,J$5&lt;=$F52+$H52-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="89" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="89" stopIfTrue="1">
       <formula>AND(LEN($C52)=0,J$5&gt;=$F52,J$5&lt;=$F52+$H52-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CA52">
-    <cfRule type="expression" dxfId="61" priority="83">
+    <cfRule type="expression" dxfId="29" priority="83">
       <formula>AND(TODAY()&gt;=CA$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J54:BZ55">
-    <cfRule type="expression" dxfId="60" priority="76">
+    <cfRule type="expression" dxfId="28" priority="76">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J54:CA55">
-    <cfRule type="expression" dxfId="59" priority="77" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="77" stopIfTrue="1">
       <formula>AND($C54="Low",J$5&gt;=$F54,J$5&lt;=$F54+$H54-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="78" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="78" stopIfTrue="1">
       <formula>AND($C54="High",J$5&gt;=$F54,J$5&lt;=$F54+$H54-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="79" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="79" stopIfTrue="1">
       <formula>AND($C54="On Track",J$5&gt;=$F54,J$5&lt;=$F54+$H54-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="80" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="80" stopIfTrue="1">
       <formula>AND($C54="Med",J$5&gt;=$F54,J$5&lt;=$F54+$H54-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="81" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="81" stopIfTrue="1">
       <formula>AND(LEN($C54)=0,J$5&gt;=$F54,J$5&lt;=$F54+$H54-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CA54:CA55">
-    <cfRule type="expression" dxfId="54" priority="75">
+    <cfRule type="expression" dxfId="22" priority="75">
       <formula>AND(TODAY()&gt;=CA$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J57:BZ63">
-    <cfRule type="expression" dxfId="53" priority="68">
+    <cfRule type="expression" dxfId="21" priority="68">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J57:CA63">
-    <cfRule type="expression" dxfId="52" priority="69" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="69" stopIfTrue="1">
       <formula>AND($C57="Low",J$5&gt;=$F57,J$5&lt;=$F57+$H57-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="70" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="70" stopIfTrue="1">
       <formula>AND($C57="High",J$5&gt;=$F57,J$5&lt;=$F57+$H57-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="71" stopIfTrue="1">
       <formula>AND($C57="On Track",J$5&gt;=$F57,J$5&lt;=$F57+$H57-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="72" stopIfTrue="1">
       <formula>AND($C57="Med",J$5&gt;=$F57,J$5&lt;=$F57+$H57-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="73" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="73" stopIfTrue="1">
       <formula>AND(LEN($C57)=0,J$5&gt;=$F57,J$5&lt;=$F57+$H57-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CA57:CA63">
-    <cfRule type="expression" dxfId="47" priority="67">
+    <cfRule type="expression" dxfId="15" priority="67">
       <formula>AND(TODAY()&gt;=CA$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J66:BZ72">
-    <cfRule type="expression" dxfId="46" priority="60">
+    <cfRule type="expression" dxfId="14" priority="60">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J66:CA72">
-    <cfRule type="expression" dxfId="45" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="61" stopIfTrue="1">
       <formula>AND($C66="Low",J$5&gt;=$F66,J$5&lt;=$F66+$H66-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="62" stopIfTrue="1">
       <formula>AND($C66="High",J$5&gt;=$F66,J$5&lt;=$F66+$H66-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="63" stopIfTrue="1">
       <formula>AND($C66="On Track",J$5&gt;=$F66,J$5&lt;=$F66+$H66-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="64" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="64" stopIfTrue="1">
       <formula>AND($C66="Med",J$5&gt;=$F66,J$5&lt;=$F66+$H66-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="65" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="65" stopIfTrue="1">
       <formula>AND(LEN($C66)=0,J$5&gt;=$F66,J$5&lt;=$F66+$H66-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CA66:CA72">
-    <cfRule type="expression" dxfId="40" priority="59">
+    <cfRule type="expression" dxfId="8" priority="59">
       <formula>AND(TODAY()&gt;=CA$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J18:BZ18">
-    <cfRule type="expression" dxfId="25" priority="32">
+    <cfRule type="expression" dxfId="7" priority="32">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CA18">
-    <cfRule type="expression" dxfId="24" priority="33">
+    <cfRule type="expression" dxfId="6" priority="33">
       <formula>AND(TODAY()&gt;=CA$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J17:BZ17">
-    <cfRule type="expression" dxfId="23" priority="29">
+    <cfRule type="expression" dxfId="5" priority="29">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CA17">
-    <cfRule type="expression" dxfId="22" priority="30">
+    <cfRule type="expression" dxfId="4" priority="30">
       <formula>AND(TODAY()&gt;=CA$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update Marching Masters Schedule.xlsx
</commit_message>
<xml_diff>
--- a/Documents/Meeting Updates/Marching Masters Schedule.xlsx
+++ b/Documents/Meeting Updates/Marching Masters Schedule.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DFE0B93-3833-154D-B8D8-8554CBDEF742}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C52D5B-9F50-5447-8D54-EE02D0953B8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20440" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="11" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="107">
   <si>
     <t>About This Template</t>
   </si>
@@ -373,6 +373,12 @@
   </si>
   <si>
     <t>Brandin/Aparna</t>
+  </si>
+  <si>
+    <t>Aparna/Tumaris</t>
+  </si>
+  <si>
+    <t>Adam/Siddharth</t>
   </si>
 </sst>
 </file>
@@ -930,6 +936,15 @@
     <xf numFmtId="14" fontId="20" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
@@ -950,15 +965,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3434,8 +3440,8 @@
   </sheetPr>
   <dimension ref="A1:CA165"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A5" zoomScaleNormal="150" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:I5"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="150" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3502,46 +3508,46 @@
       <c r="F2" s="23"/>
       <c r="G2" s="23"/>
       <c r="H2" s="21"/>
-      <c r="J2" s="67" t="s">
+      <c r="J2" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="67"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="67"/>
-      <c r="Q2" s="68" t="s">
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="70"/>
+      <c r="O2" s="70"/>
+      <c r="Q2" s="71" t="s">
         <v>51</v>
       </c>
-      <c r="R2" s="68"/>
-      <c r="S2" s="68"/>
-      <c r="T2" s="68"/>
-      <c r="U2" s="68"/>
-      <c r="V2" s="68"/>
-      <c r="X2" s="69" t="s">
+      <c r="R2" s="71"/>
+      <c r="S2" s="71"/>
+      <c r="T2" s="71"/>
+      <c r="U2" s="71"/>
+      <c r="V2" s="71"/>
+      <c r="X2" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="Y2" s="69"/>
-      <c r="Z2" s="69"/>
-      <c r="AA2" s="69"/>
-      <c r="AB2" s="69"/>
-      <c r="AC2" s="69"/>
-      <c r="AE2" s="70" t="s">
+      <c r="Y2" s="61"/>
+      <c r="Z2" s="61"/>
+      <c r="AA2" s="61"/>
+      <c r="AB2" s="61"/>
+      <c r="AC2" s="61"/>
+      <c r="AE2" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="AF2" s="70"/>
-      <c r="AG2" s="70"/>
-      <c r="AH2" s="70"/>
-      <c r="AI2" s="70"/>
-      <c r="AJ2" s="70"/>
-      <c r="AL2" s="71" t="s">
+      <c r="AF2" s="62"/>
+      <c r="AG2" s="62"/>
+      <c r="AH2" s="62"/>
+      <c r="AI2" s="62"/>
+      <c r="AJ2" s="62"/>
+      <c r="AL2" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="AM2" s="71"/>
-      <c r="AN2" s="71"/>
-      <c r="AO2" s="71"/>
-      <c r="AP2" s="71"/>
-      <c r="AQ2" s="71"/>
+      <c r="AM2" s="63"/>
+      <c r="AN2" s="63"/>
+      <c r="AO2" s="63"/>
+      <c r="AP2" s="63"/>
+      <c r="AQ2" s="63"/>
       <c r="AR2" s="20"/>
       <c r="AW2" s="20"/>
       <c r="BB2" s="20"/>
@@ -3552,26 +3558,26 @@
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
-      <c r="D3" s="61" t="s">
+      <c r="D3" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="62"/>
-      <c r="F3" s="64">
+      <c r="E3" s="65"/>
+      <c r="F3" s="67">
         <f ca="1">IFERROR(IF(MIN(Milestones[Start])=0,TODAY(),MIN(Milestones[Start])),TODAY())</f>
         <v>44096</v>
       </c>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="69"/>
       <c r="I3" s="22"/>
     </row>
     <row r="4" spans="1:79" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="61" t="s">
+      <c r="D4" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="62"/>
+      <c r="E4" s="65"/>
       <c r="F4" s="39">
         <v>21</v>
       </c>
@@ -3675,14 +3681,14 @@
       <c r="A5" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="63"/>
-      <c r="I5" s="63"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="66"/>
       <c r="J5" s="43">
         <f ca="1">IFERROR(Project_Start+Scrolling_Increment,TODAY())</f>
         <v>44117</v>
@@ -6164,7 +6170,7 @@
         <v>52</v>
       </c>
       <c r="D14" s="48" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="E14" s="29">
         <v>0</v>
@@ -9997,7 +10003,9 @@
       <c r="C35" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="D35" s="48"/>
+      <c r="D35" s="48" t="s">
+        <v>106</v>
+      </c>
       <c r="E35" s="56">
         <v>0</v>
       </c>
@@ -16258,15 +16266,15 @@
     <row r="165" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B5:I5"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="J2:O2"/>
+    <mergeCell ref="Q2:V2"/>
     <mergeCell ref="X2:AC2"/>
     <mergeCell ref="AE2:AJ2"/>
     <mergeCell ref="AL2:AQ2"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="D4:E4"/>
-    <mergeCell ref="B5:I5"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="J2:O2"/>
-    <mergeCell ref="Q2:V2"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:E11 E16 E13:E14 E53 E23:E24 E64:E65 E72 E33 E69">
     <cfRule type="dataBar" priority="339">

</xml_diff>